<commit_message>
performance optimisation, structure, requirements
</commit_message>
<xml_diff>
--- a/Output/portfolio_overview.xlsx
+++ b/Output/portfolio_overview.xlsx
@@ -20,8 +20,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.00%;(-0.00%)"/>
-    <numFmt numFmtId="165" formatCode="0.00;(-0.00)"/>
+    <numFmt numFmtId="164" formatCode="0.00%;-0.00%"/>
+    <numFmt numFmtId="165" formatCode="0.00;-0.00"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -177,7 +177,7 @@
     <tableColumn id="2" name="weight"/>
     <tableColumn id="3" name="total_return"/>
     <tableColumn id="4" name="relative_return"/>
-    <tableColumn id="5" name="volatility"/>
+    <tableColumn id="5" name="volatility_annualised"/>
     <tableColumn id="6" name="beta"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showRowStripes="1"/>
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3068100870144</v>
+        <v>3030152118272</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2788063707136</v>
+        <v>2754544140288</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>257685110784</v>
+        <v>257525006336</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>173891911680</v>
+        <v>172966952960</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>69121925120</v>
+        <v>68716519424</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>85422997504</v>
+        <v>85067333632</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -696,7 +696,7 @@
     <col width="25.27" customWidth="1" min="2" max="2"/>
     <col width="26.6" customWidth="1" min="3" max="3"/>
     <col width="26.6" customWidth="1" min="4" max="4"/>
-    <col width="26.6" customWidth="1" min="5" max="5"/>
+    <col width="27.93" customWidth="1" min="5" max="5"/>
     <col width="25.27" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -721,9 +721,9 @@
           <t>relative_return</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>volatility</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>volatility_annualised</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
@@ -742,16 +742,16 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.5272386858268681</v>
+        <v>0.5272385921430498</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.2785968373582619</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0.0128681548244216</v>
+        <v>0.2785967589266225</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.2042756207379944</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>1.135231052693318</v>
+        <v>1.135230519657438</v>
       </c>
     </row>
     <row r="3">
@@ -764,16 +764,16 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.5955829673719613</v>
+        <v>0.5955828648486217</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.3358143391450028</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0.01627271126854903</v>
+        <v>0.3358142533129591</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.2583213308381355</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>1.231811932306462</v>
+        <v>1.231812313596667</v>
       </c>
     </row>
     <row r="4">
@@ -791,8 +791,8 @@
       <c r="D4" s="1" t="n">
         <v>-0.2164889328306131</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>0.00945246791101406</v>
+      <c r="E4" t="n">
+        <v>0.1500532762101685</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0.1006726915775444</v>
@@ -813,8 +813,8 @@
       <c r="D5" s="1" t="n">
         <v>-0.08467792058680756</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>0.01143420621841345</v>
+      <c r="E5" t="n">
+        <v>0.1815123965601017</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0.07353444126260401</v>
@@ -835,8 +835,8 @@
       <c r="D6" s="1" t="n">
         <v>0.04043873036511303</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>0.01370483143133685</v>
+      <c r="E6" t="n">
+        <v>0.2175574543642721</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4945557085830209</v>
@@ -857,8 +857,8 @@
       <c r="D7" s="1" t="n">
         <v>0.1927631354793895</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>0.01927952566603645</v>
+      <c r="E7" t="n">
+        <v>0.3060529818457162</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.8353580271976099</v>
@@ -890,7 +890,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.3" customWidth="1" min="1" max="1"/>
-    <col width="27.93" customWidth="1" min="2" max="2"/>
+    <col width="29.26" customWidth="1" min="2" max="2"/>
     <col width="27.93" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -944,7 +944,7 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.006612910024253127</v>
+        <v>0.006612900163591728</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0.007538970575044379</v>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>-0.002080993535229392</v>
+        <v>-0.002080993877223825</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>-0.004194353599094369</v>
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.01084165251570024</v>
+        <v>0.01084163990121034</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.01855062511822725</v>
@@ -983,7 +983,7 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0.01777196698180883</v>
+        <v>0.01777195742856974</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0.01776875250938836</v>
@@ -996,7 +996,7 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.01478155934491365</v>
+        <v>0.01478153823481443</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.02487098016640643</v>
@@ -1009,7 +1009,7 @@
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.03341213256992792</v>
+        <v>0.03341211107226427</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.03803998256603447</v>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0.04018879116180107</v>
+        <v>0.04018874972548403</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0.04158582943200351</v>
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.04343309637769899</v>
+        <v>0.04343308614280894</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0.04574890046570768</v>
@@ -1048,7 +1048,7 @@
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>0.05273370783923848</v>
+        <v>0.05273369751311985</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0.04574890046570768</v>
@@ -1061,7 +1061,7 @@
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.05621999387753029</v>
+        <v>0.05621999215182716</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.04362551653740021</v>
@@ -1074,7 +1074,7 @@
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.0463442357170496</v>
+        <v>0.04634423411418287</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0.02738399163874461</v>
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.03448887219488239</v>
+        <v>0.03448887060139283</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.01953647282180282</v>
@@ -1100,7 +1100,7 @@
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.04836728227574105</v>
+        <v>0.04836726072744102</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.03882447269565104</v>
@@ -1113,7 +1113,7 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.06164292719610587</v>
+        <v>0.06164289712594018</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.05116710463322227</v>
@@ -1126,7 +1126,7 @@
         </is>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.06189513567031524</v>
+        <v>0.06189511382323132</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0.05041919595252109</v>
@@ -1139,7 +1139,7 @@
         </is>
       </c>
       <c r="B19" s="1" t="n">
-        <v>0.05897099573388376</v>
+        <v>0.05897097394696016</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0.05022830846167192</v>
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>0.06184316820088887</v>
+        <v>0.06184316544521473</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.06178906779040427</v>
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>0.06403372366620408</v>
+        <v>0.06403369390624136</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0.06443806265923357</v>
@@ -1178,7 +1178,7 @@
         </is>
       </c>
       <c r="B22" s="1" t="n">
-        <v>0.06186365992379561</v>
+        <v>0.06186363773751813</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0.05063364113036783</v>
@@ -1191,7 +1191,7 @@
         </is>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.06094310744034814</v>
+        <v>0.06094308527330439</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>0.06601751300157654</v>
@@ -1204,7 +1204,7 @@
         </is>
       </c>
       <c r="B24" s="1" t="n">
-        <v>0.06287620218624923</v>
+        <v>0.0628761611750237</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>0.07715985205772524</v>
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="B25" s="1" t="n">
-        <v>0.06896955973565189</v>
+        <v>0.06896953787241333</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>0.09299342676690747</v>
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="B26" s="1" t="n">
-        <v>0.08239083502262989</v>
+        <v>0.08239081288489092</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>0.08167590534457481</v>
@@ -1243,7 +1243,7 @@
         </is>
       </c>
       <c r="B27" s="1" t="n">
-        <v>0.07149576628055598</v>
+        <v>0.07149574436564987</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>0.07503391445061047</v>
@@ -1256,7 +1256,7 @@
         </is>
       </c>
       <c r="B28" s="1" t="n">
-        <v>0.07876174859149998</v>
+        <v>0.07876174458760343</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>0.08887229990761392</v>
@@ -1269,7 +1269,7 @@
         </is>
       </c>
       <c r="B29" s="1" t="n">
-        <v>0.07586912100167686</v>
+        <v>0.07586909948463849</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>0.07680680596260991</v>
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B30" s="1" t="n">
-        <v>0.07434485099303467</v>
+        <v>0.07434482950648125</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>0.06729882134316201</v>
@@ -1295,7 +1295,7 @@
         </is>
       </c>
       <c r="B31" s="1" t="n">
-        <v>0.07177656522082065</v>
+        <v>0.07177650466265284</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>0.0696418216489012</v>
@@ -1308,7 +1308,7 @@
         </is>
       </c>
       <c r="B32" s="1" t="n">
-        <v>0.08713298308412964</v>
+        <v>0.08713296167836337</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0.08188773300164431</v>
@@ -1321,7 +1321,7 @@
         </is>
       </c>
       <c r="B33" s="1" t="n">
-        <v>0.08873637123646594</v>
+        <v>0.0887363497991287</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>0.08158435595933167</v>
@@ -1334,7 +1334,7 @@
         </is>
       </c>
       <c r="B34" s="1" t="n">
-        <v>0.09373301153430225</v>
+        <v>0.09373300814499963</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>0.08458377940249884</v>
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="B35" s="1" t="n">
-        <v>0.07891828808880419</v>
+        <v>0.07891826695320492</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>0.06962873404501346</v>
@@ -1360,7 +1360,7 @@
         </is>
       </c>
       <c r="B36" s="1" t="n">
-        <v>0.07833377728751101</v>
+        <v>0.07833375616336213</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>0.06666863725547945</v>
@@ -1373,7 +1373,7 @@
         </is>
       </c>
       <c r="B37" s="1" t="n">
-        <v>0.076552420926149</v>
+        <v>0.07655239983689621</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>0.06666863725547945</v>
@@ -1386,7 +1386,7 @@
         </is>
       </c>
       <c r="B38" s="1" t="n">
-        <v>0.06870892573964515</v>
+        <v>0.06870890480404346</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>0.04529128122343162</v>
@@ -1399,7 +1399,7 @@
         </is>
       </c>
       <c r="B39" s="1" t="n">
-        <v>0.06822472241648447</v>
+        <v>0.06822470149036808</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>0.04364645670362055</v>
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B40" s="1" t="n">
-        <v>0.0698845389974021</v>
+        <v>0.06988449972129152</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>0.04920849682995865</v>
@@ -1425,7 +1425,7 @@
         </is>
       </c>
       <c r="B41" s="1" t="n">
-        <v>0.06001695861933265</v>
+        <v>0.06001691937622633</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>0.03815240827552802</v>
@@ -1438,7 +1438,7 @@
         </is>
       </c>
       <c r="B42" s="1" t="n">
-        <v>0.06571898797714448</v>
+        <v>0.06571898557371236</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>0.0413426553675742</v>
@@ -1451,7 +1451,7 @@
         </is>
       </c>
       <c r="B43" s="1" t="n">
-        <v>0.0587047578645199</v>
+        <v>0.05870475554033461</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>0.03818113716211058</v>
@@ -1464,7 +1464,7 @@
         </is>
       </c>
       <c r="B44" s="1" t="n">
-        <v>0.05151449238686268</v>
+        <v>0.05151447947646703</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>0.0332754563312303</v>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="B45" s="1" t="n">
-        <v>0.06089637870325992</v>
+        <v>0.06089635826596562</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>0.04110995138625473</v>
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="B46" s="1" t="n">
-        <v>0.07442551625252092</v>
+        <v>0.07442552493292798</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>0.05792152123667993</v>
@@ -1503,7 +1503,7 @@
         </is>
       </c>
       <c r="B47" s="1" t="n">
-        <v>0.0758340077129922</v>
+        <v>0.0758339870650806</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>0.05864848975116099</v>
@@ -1516,7 +1516,7 @@
         </is>
       </c>
       <c r="B48" s="1" t="n">
-        <v>0.06756329497379054</v>
+        <v>0.06756327448461441</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>0.04242266997717059</v>
@@ -1529,7 +1529,7 @@
         </is>
       </c>
       <c r="B49" s="1" t="n">
-        <v>0.06677416631834343</v>
+        <v>0.06677413509403163</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>0.04389748333038268</v>
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="B50" s="1" t="n">
-        <v>0.06536571053051099</v>
+        <v>0.06536569005027659</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>0.02462780610197712</v>
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B51" s="1" t="n">
-        <v>0.04296911764190958</v>
+        <v>0.0429690975922199</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>0.009793102858287828</v>
@@ -1568,7 +1568,7 @@
         </is>
       </c>
       <c r="B52" s="1" t="n">
-        <v>0.03289152762278902</v>
+        <v>0.03289152570061304</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>0.00826855661030268</v>
@@ -1581,7 +1581,7 @@
         </is>
       </c>
       <c r="B53" s="1" t="n">
-        <v>0.05141985747860423</v>
+        <v>0.05141981692589637</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>0.02488145024951671</v>
@@ -1594,7 +1594,7 @@
         </is>
       </c>
       <c r="B54" s="1" t="n">
-        <v>0.03274318550145994</v>
+        <v>0.03274316363155916</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>0.01772687217694791</v>
@@ -1607,7 +1607,7 @@
         </is>
       </c>
       <c r="B55" s="1" t="n">
-        <v>0.0608588027394481</v>
+        <v>0.06085880335167415</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>0.03560019783349699</v>
@@ -1620,7 +1620,7 @@
         </is>
       </c>
       <c r="B56" s="1" t="n">
-        <v>0.05508451603639331</v>
+        <v>0.05508451641537682</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>0.02418844566317313</v>
@@ -1633,7 +1633,7 @@
         </is>
       </c>
       <c r="B57" s="1" t="n">
-        <v>0.05860876631549172</v>
+        <v>0.05860874786690551</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>0.0333225717052259</v>
@@ -1646,7 +1646,7 @@
         </is>
       </c>
       <c r="B58" s="1" t="n">
-        <v>0.08499172287834367</v>
+        <v>0.08499168679651947</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>0.04673736569006093</v>
@@ -1659,7 +1659,7 @@
         </is>
       </c>
       <c r="B59" s="1" t="n">
-        <v>0.0784515103716652</v>
+        <v>0.07845149174270394</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>0.02950469420430446</v>
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="B60" s="1" t="n">
-        <v>0.07361691887841038</v>
+        <v>0.07361688288526747</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>0.03257728054530196</v>
@@ -1685,7 +1685,7 @@
         </is>
       </c>
       <c r="B61" s="1" t="n">
-        <v>0.06630821175763701</v>
+        <v>0.06630821065130377</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>0.03840081738151224</v>
@@ -1698,7 +1698,7 @@
         </is>
       </c>
       <c r="B62" s="1" t="n">
-        <v>0.07986706716465508</v>
+        <v>0.07986704926241051</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>0.0401110160787912</v>
@@ -1711,7 +1711,7 @@
         </is>
       </c>
       <c r="B63" s="1" t="n">
-        <v>0.08725480879457326</v>
+        <v>0.08725477334892817</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>0.03847404412131272</v>
@@ -1724,7 +1724,7 @@
         </is>
       </c>
       <c r="B64" s="1" t="n">
-        <v>0.1049084403615979</v>
+        <v>0.1049084020791191</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>0.05325907831219889</v>
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="B65" s="1" t="n">
-        <v>0.1185439047508965</v>
+        <v>0.1185439039608092</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>0.05927873768081326</v>
@@ -1750,7 +1750,7 @@
         </is>
       </c>
       <c r="B66" s="1" t="n">
-        <v>0.1323023193009456</v>
+        <v>0.1323023207905214</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>0.07457106016677861</v>
@@ -1763,7 +1763,7 @@
         </is>
       </c>
       <c r="B67" s="1" t="n">
-        <v>0.1301663938142976</v>
+        <v>0.1301663577390231</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>0.07854573354647099</v>
@@ -1776,7 +1776,7 @@
         </is>
       </c>
       <c r="B68" s="1" t="n">
-        <v>0.1270056201498766</v>
+        <v>0.1270056188524098</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>0.07229343403850752</v>
@@ -1789,7 +1789,7 @@
         </is>
       </c>
       <c r="B69" s="1" t="n">
-        <v>0.1207901136515974</v>
+        <v>0.1207900951828804</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>0.06962088148268042</v>
@@ -1802,7 +1802,7 @@
         </is>
       </c>
       <c r="B70" s="1" t="n">
-        <v>0.1308468126451343</v>
+        <v>0.1308467940106999</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>0.07344922906671192</v>
@@ -1815,7 +1815,7 @@
         </is>
       </c>
       <c r="B71" s="1" t="n">
-        <v>0.1308468126451343</v>
+        <v>0.1308467940106999</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>0.07344922906671192</v>
@@ -1828,7 +1828,7 @@
         </is>
       </c>
       <c r="B72" s="1" t="n">
-        <v>0.1264080339094091</v>
+        <v>0.126407997811631</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>0.0745187097512281</v>
@@ -1841,7 +1841,7 @@
         </is>
       </c>
       <c r="B73" s="1" t="n">
-        <v>0.1266629695653114</v>
+        <v>0.1266629709989628</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>0.07447427573998033</v>
@@ -1854,7 +1854,7 @@
         </is>
       </c>
       <c r="B74" s="1" t="n">
-        <v>0.1340977286054164</v>
+        <v>0.1340977096110567</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>0.07003144919293147</v>
@@ -1867,7 +1867,7 @@
         </is>
       </c>
       <c r="B75" s="1" t="n">
-        <v>0.1426214563831114</v>
+        <v>0.1426214372459929</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>0.08422294458702062</v>
@@ -1880,7 +1880,7 @@
         </is>
       </c>
       <c r="B76" s="1" t="n">
-        <v>0.1509842201400085</v>
+        <v>0.1509841806842591</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>0.08197928238688723</v>
@@ -1893,7 +1893,7 @@
         </is>
       </c>
       <c r="B77" s="1" t="n">
-        <v>0.1490113999614264</v>
+        <v>0.1490113607647041</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>0.08555647566021629</v>
@@ -1906,7 +1906,7 @@
         </is>
       </c>
       <c r="B78" s="1" t="n">
-        <v>0.1517258603960061</v>
+        <v>0.1517258591975521</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>0.08648486559062674</v>
@@ -1919,7 +1919,7 @@
         </is>
       </c>
       <c r="B79" s="1" t="n">
-        <v>0.1509651859754619</v>
+        <v>0.1509651465455883</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>0.08639331620538337</v>
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="B80" s="1" t="n">
-        <v>0.1453260038848114</v>
+        <v>0.1453259820146751</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>0.07992650767760279</v>
@@ -1945,7 +1945,7 @@
         </is>
       </c>
       <c r="B81" s="1" t="n">
-        <v>0.1454623639825516</v>
+        <v>0.1454623627464147</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>0.0809018852980683</v>
@@ -1958,7 +1958,7 @@
         </is>
       </c>
       <c r="B82" s="1" t="n">
-        <v>0.1487350729288548</v>
+        <v>0.1487350744490605</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>0.08182235882417599</v>
@@ -1971,7 +1971,7 @@
         </is>
       </c>
       <c r="B83" s="1" t="n">
-        <v>0.1543254141183572</v>
+        <v>0.1543254161162309</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>0.06471781817257805</v>
@@ -1984,7 +1984,7 @@
         </is>
       </c>
       <c r="B84" s="1" t="n">
-        <v>0.1611153603814426</v>
+        <v>0.1611153393846054</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>0.06062803772064451</v>
@@ -1997,7 +1997,7 @@
         </is>
       </c>
       <c r="B85" s="1" t="n">
-        <v>0.1716849313657256</v>
+        <v>0.1716848900564905</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>0.08138044470656491</v>
@@ -2010,7 +2010,7 @@
         </is>
       </c>
       <c r="B86" s="1" t="n">
-        <v>0.1762257860443732</v>
+        <v>0.1762257821713817</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>0.09030529677035548</v>
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="B87" s="1" t="n">
-        <v>0.1750371675945404</v>
+        <v>0.1750371637348505</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>0.08988432281896475</v>
@@ -2036,7 +2036,7 @@
         </is>
       </c>
       <c r="B88" s="1" t="n">
-        <v>0.1710239813845316</v>
+        <v>0.1710239599555066</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>0.07725663648452352</v>
@@ -2049,7 +2049,7 @@
         </is>
       </c>
       <c r="B89" s="1" t="n">
-        <v>0.1679387719243397</v>
+        <v>0.1679387505517722</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>0.06971766590947914</v>
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B90" s="1" t="n">
-        <v>0.1586826303745907</v>
+        <v>0.1586826091714049</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>0.0619956604059182</v>
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="B91" s="1" t="n">
-        <v>0.183078762875845</v>
+        <v>0.1830787427995726</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>0.08161576620866162</v>
@@ -2088,7 +2088,7 @@
         </is>
       </c>
       <c r="B92" s="1" t="n">
-        <v>0.184609738689318</v>
+        <v>0.1846096797186623</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>0.08210479570026807</v>
@@ -2101,7 +2101,7 @@
         </is>
       </c>
       <c r="B93" s="1" t="n">
-        <v>0.1827438841549296</v>
+        <v>0.1827438424325263</v>
       </c>
       <c r="C93" s="1" t="n">
         <v>0.07714938197461474</v>
@@ -2114,7 +2114,7 @@
         </is>
       </c>
       <c r="B94" s="1" t="n">
-        <v>0.180276956007124</v>
+        <v>0.1802769344324437</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>0.08197928238688701</v>
@@ -2127,7 +2127,7 @@
         </is>
       </c>
       <c r="B95" s="1" t="n">
-        <v>0.1821338002282156</v>
+        <v>0.1821337786195933</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>0.08014357037622699</v>
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="B96" s="1" t="n">
-        <v>0.1820045569610709</v>
+        <v>0.1820045179820531</v>
       </c>
       <c r="C96" s="1" t="n">
         <v>0.07843337167894782</v>
@@ -2153,7 +2153,7 @@
         </is>
       </c>
       <c r="B97" s="1" t="n">
-        <v>0.1813364258464201</v>
+        <v>0.18133640430431</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>0.08162355492902362</v>
@@ -2166,7 +2166,7 @@
         </is>
       </c>
       <c r="B98" s="1" t="n">
-        <v>0.1803118074935575</v>
+        <v>0.1803117859701318</v>
       </c>
       <c r="C98" s="1" t="n">
         <v>0.07472530236674202</v>
@@ -2179,7 +2179,7 @@
         </is>
       </c>
       <c r="B99" s="1" t="n">
-        <v>0.1810470943699631</v>
+        <v>0.181047072833129</v>
       </c>
       <c r="C99" s="1" t="n">
         <v>0.08750467722233957</v>
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="B100" s="1" t="n">
-        <v>0.1865706525742155</v>
+        <v>0.186570613497453</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>0.09777621180518348</v>
@@ -2205,7 +2205,7 @@
         </is>
       </c>
       <c r="B101" s="1" t="n">
-        <v>0.198222101136281</v>
+        <v>0.1982220789712219</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>0.09618897274247806</v>
@@ -2218,7 +2218,7 @@
         </is>
       </c>
       <c r="B102" s="1" t="n">
-        <v>0.1988314908091608</v>
+        <v>0.1988314686328292</v>
       </c>
       <c r="C102" s="1" t="n">
         <v>0.09635892006710689</v>
@@ -2231,7 +2231,7 @@
         </is>
       </c>
       <c r="B103" s="1" t="n">
-        <v>0.1880644817121517</v>
+        <v>0.1880644597349914</v>
       </c>
       <c r="C103" s="1" t="n">
         <v>0.08405555094119865</v>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="B104" s="1" t="n">
-        <v>0.1809656431667943</v>
+        <v>0.1809656213209505</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>0.0761217816225388</v>
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="B105" s="1" t="n">
-        <v>0.1841688711755682</v>
+        <v>0.1841688492704701</v>
       </c>
       <c r="C105" s="1" t="n">
         <v>0.08554600557710579</v>
@@ -2270,7 +2270,7 @@
         </is>
       </c>
       <c r="B106" s="1" t="n">
-        <v>0.1991529200751725</v>
+        <v>0.1991529153478724</v>
       </c>
       <c r="C106" s="1" t="n">
         <v>0.09971138960538983</v>
@@ -2283,7 +2283,7 @@
         </is>
       </c>
       <c r="B107" s="1" t="n">
-        <v>0.1991529200751725</v>
+        <v>0.1991529153478724</v>
       </c>
       <c r="C107" s="1" t="n">
         <v>0.09971138960538983</v>
@@ -2296,7 +2296,7 @@
         </is>
       </c>
       <c r="B108" s="1" t="n">
-        <v>0.1855950011578342</v>
+        <v>0.1855949788681859</v>
       </c>
       <c r="C108" s="1" t="n">
         <v>0.09972964840886234</v>
@@ -2309,7 +2309,7 @@
         </is>
       </c>
       <c r="B109" s="1" t="n">
-        <v>0.1770286260950156</v>
+        <v>0.177028621017592</v>
       </c>
       <c r="C109" s="1" t="n">
         <v>0.09301181325431984</v>
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="B110" s="1" t="n">
-        <v>0.1925560733194787</v>
+        <v>0.1925560509710189</v>
       </c>
       <c r="C110" s="1" t="n">
         <v>0.1037828474118807</v>
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="B111" s="1" t="n">
-        <v>0.2069206666662466</v>
+        <v>0.2069206440485949</v>
       </c>
       <c r="C111" s="1" t="n">
         <v>0.1198256960993249</v>
@@ -2348,7 +2348,7 @@
         </is>
       </c>
       <c r="B112" s="1" t="n">
-        <v>0.2069869151298849</v>
+        <v>0.2069868925109917</v>
       </c>
       <c r="C112" s="1" t="n">
         <v>0.1175820338991915</v>
@@ -2361,7 +2361,7 @@
         </is>
       </c>
       <c r="B113" s="1" t="n">
-        <v>0.2081463733810223</v>
+        <v>0.2081463678788396</v>
       </c>
       <c r="C113" s="1" t="n">
         <v>0.120212706122578</v>
@@ -2374,7 +2374,7 @@
         </is>
       </c>
       <c r="B114" s="1" t="n">
-        <v>0.1962757606030867</v>
+        <v>0.1962757380979776</v>
       </c>
       <c r="C114" s="1" t="n">
         <v>0.1159424444209354</v>
@@ -2387,7 +2387,7 @@
         </is>
       </c>
       <c r="B115" s="1" t="n">
-        <v>0.2015949219993305</v>
+        <v>0.2015948993941539</v>
       </c>
       <c r="C115" s="1" t="n">
         <v>0.1228486133875195</v>
@@ -2400,7 +2400,7 @@
         </is>
       </c>
       <c r="B116" s="1" t="n">
-        <v>0.204186314087905</v>
+        <v>0.2041862914339776</v>
       </c>
       <c r="C116" s="1" t="n">
         <v>0.1241377104494672</v>
@@ -2413,7 +2413,7 @@
         </is>
       </c>
       <c r="B117" s="1" t="n">
-        <v>0.2149338509620817</v>
+        <v>0.2149338450742422</v>
       </c>
       <c r="C117" s="1" t="n">
         <v>0.134615965331766</v>
@@ -2426,7 +2426,7 @@
         </is>
       </c>
       <c r="B118" s="1" t="n">
-        <v>0.2166333112696295</v>
+        <v>0.2166332717053492</v>
       </c>
       <c r="C118" s="1" t="n">
         <v>0.1424816791102101</v>
@@ -2439,7 +2439,7 @@
         </is>
       </c>
       <c r="B119" s="1" t="n">
-        <v>0.2195718484973537</v>
+        <v>0.2195718258204917</v>
       </c>
       <c r="C119" s="1" t="n">
         <v>0.1434178577609828</v>
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="B120" s="1" t="n">
-        <v>0.230427874681731</v>
+        <v>0.2304278687087535</v>
       </c>
       <c r="C120" s="1" t="n">
         <v>0.1573425575616745</v>
@@ -2465,7 +2465,7 @@
         </is>
       </c>
       <c r="B121" s="1" t="n">
-        <v>0.2270374754285365</v>
+        <v>0.2270374527035213</v>
       </c>
       <c r="C121" s="1" t="n">
         <v>0.1530932360262522</v>
@@ -2478,7 +2478,7 @@
         </is>
       </c>
       <c r="B122" s="1" t="n">
-        <v>0.2285436140083743</v>
+        <v>0.2285435912554652</v>
       </c>
       <c r="C122" s="1" t="n">
         <v>0.1530932360262522</v>
@@ -2491,7 +2491,7 @@
         </is>
       </c>
       <c r="B123" s="1" t="n">
-        <v>0.2166679324980068</v>
+        <v>0.2166679099650382</v>
       </c>
       <c r="C123" s="1" t="n">
         <v>0.1476332153682676</v>
@@ -2504,7 +2504,7 @@
         </is>
       </c>
       <c r="B124" s="1" t="n">
-        <v>0.2128756029656333</v>
+        <v>0.2128755805028997</v>
       </c>
       <c r="C124" s="1" t="n">
         <v>0.1416135559996532</v>
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="B125" s="1" t="n">
-        <v>0.2158843371192198</v>
+        <v>0.2158842977887589</v>
       </c>
       <c r="C125" s="1" t="n">
         <v>0.1458498537731581</v>
@@ -2530,7 +2530,7 @@
         </is>
       </c>
       <c r="B126" s="1" t="n">
-        <v>0.2130905811880137</v>
+        <v>0.2130905584992746</v>
       </c>
       <c r="C126" s="1" t="n">
         <v>0.137074008867776</v>
@@ -2543,7 +2543,7 @@
         </is>
       </c>
       <c r="B127" s="1" t="n">
-        <v>0.2008828858743643</v>
+        <v>0.2008828468439634</v>
       </c>
       <c r="C127" s="1" t="n">
         <v>0.1319721416625215</v>
@@ -2556,7 +2556,7 @@
         </is>
       </c>
       <c r="B128" s="1" t="n">
-        <v>0.2091656384925242</v>
+        <v>0.2091656159698905</v>
       </c>
       <c r="C128" s="1" t="n">
         <v>0.1449398503301607</v>
@@ -2569,7 +2569,7 @@
         </is>
       </c>
       <c r="B129" s="1" t="n">
-        <v>0.2126337831125313</v>
+        <v>0.2126337605252977</v>
       </c>
       <c r="C129" s="1" t="n">
         <v>0.1445344538194946</v>
@@ -2582,7 +2582,7 @@
         </is>
       </c>
       <c r="B130" s="1" t="n">
-        <v>0.2122480641062459</v>
+        <v>0.2122480415261967</v>
       </c>
       <c r="C130" s="1" t="n">
         <v>0.1496545798282216</v>
@@ -2595,7 +2595,7 @@
         </is>
       </c>
       <c r="B131" s="1" t="n">
-        <v>0.2299601541236014</v>
+        <v>0.2299601149093136</v>
       </c>
       <c r="C131" s="1" t="n">
         <v>0.1637596970366524</v>
@@ -2608,7 +2608,7 @@
         </is>
       </c>
       <c r="B132" s="1" t="n">
-        <v>0.2227355640566175</v>
+        <v>0.2227355411157961</v>
       </c>
       <c r="C132" s="1" t="n">
         <v>0.1651220846803712</v>
@@ -2621,7 +2621,7 @@
         </is>
       </c>
       <c r="B133" s="1" t="n">
-        <v>0.219811647803704</v>
+        <v>0.2198116249177409</v>
       </c>
       <c r="C133" s="1" t="n">
         <v>0.1651220846803712</v>
@@ -2634,7 +2634,7 @@
         </is>
       </c>
       <c r="B134" s="1" t="n">
-        <v>0.2151920899426587</v>
+        <v>0.2151920671433671</v>
       </c>
       <c r="C134" s="1" t="n">
         <v>0.1628287534274349</v>
@@ -2647,7 +2647,7 @@
         </is>
       </c>
       <c r="B135" s="1" t="n">
-        <v>0.2023788737935861</v>
+        <v>0.2023788512346947</v>
       </c>
       <c r="C135" s="1" t="n">
         <v>0.1536162294459968</v>
@@ -2660,7 +2660,7 @@
         </is>
       </c>
       <c r="B136" s="1" t="n">
-        <v>0.193224774669311</v>
+        <v>0.1932247522821677</v>
       </c>
       <c r="C136" s="1" t="n">
         <v>0.15031100296565</v>
@@ -2673,7 +2673,7 @@
         </is>
       </c>
       <c r="B137" s="1" t="n">
-        <v>0.1921795723086732</v>
+        <v>0.1921795499411398</v>
       </c>
       <c r="C137" s="1" t="n">
         <v>0.1530775309015873</v>
@@ -2686,7 +2686,7 @@
         </is>
       </c>
       <c r="B138" s="1" t="n">
-        <v>0.1922878360808347</v>
+        <v>0.1922877975935502</v>
       </c>
       <c r="C138" s="1" t="n">
         <v>0.1608518229787286</v>
@@ -2699,7 +2699,7 @@
         </is>
       </c>
       <c r="B139" s="1" t="n">
-        <v>0.2008750479284493</v>
+        <v>0.2008750254738216</v>
       </c>
       <c r="C139" s="1" t="n">
         <v>0.1694551668806745</v>
@@ -2712,7 +2712,7 @@
         </is>
       </c>
       <c r="B140" s="1" t="n">
-        <v>0.2039303067439051</v>
+        <v>0.2039303003681869</v>
       </c>
       <c r="C140" s="1" t="n">
         <v>0.1793606316064857</v>
@@ -2725,7 +2725,7 @@
         </is>
       </c>
       <c r="B141" s="1" t="n">
-        <v>0.207008502080702</v>
+        <v>0.2070084956759974</v>
       </c>
       <c r="C141" s="1" t="n">
         <v>0.1781524861627306</v>
@@ -2738,7 +2738,7 @@
         </is>
       </c>
       <c r="B142" s="1" t="n">
-        <v>0.2091184872658129</v>
+        <v>0.2091184482901844</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>0.1826947146573554</v>
@@ -2751,7 +2751,7 @@
         </is>
       </c>
       <c r="B143" s="1" t="n">
-        <v>0.2284148265136039</v>
+        <v>0.2284148027880373</v>
       </c>
       <c r="C143" s="1" t="n">
         <v>0.191112278426067</v>
@@ -2764,7 +2764,7 @@
         </is>
       </c>
       <c r="B144" s="1" t="n">
-        <v>0.2252056214110214</v>
+        <v>0.2252055977474372</v>
       </c>
       <c r="C144" s="1" t="n">
         <v>0.1939208143783853</v>
@@ -2777,7 +2777,7 @@
         </is>
       </c>
       <c r="B145" s="1" t="n">
-        <v>0.228881291015028</v>
+        <v>0.2288812672804521</v>
       </c>
       <c r="C145" s="1" t="n">
         <v>0.1858536153420414</v>
@@ -2790,7 +2790,7 @@
         </is>
       </c>
       <c r="B146" s="1" t="n">
-        <v>0.2307000871833371</v>
+        <v>0.2307000634136331</v>
       </c>
       <c r="C146" s="1" t="n">
         <v>0.1862379440025468</v>
@@ -2803,7 +2803,7 @@
         </is>
       </c>
       <c r="B147" s="1" t="n">
-        <v>0.2336397336382814</v>
+        <v>0.2336397098118013</v>
       </c>
       <c r="C147" s="1" t="n">
         <v>0.1910234104035713</v>
@@ -2816,7 +2816,7 @@
         </is>
       </c>
       <c r="B148" s="1" t="n">
-        <v>0.2403392793638643</v>
+        <v>0.2403392390879715</v>
       </c>
       <c r="C148" s="1" t="n">
         <v>0.1943757522579137</v>
@@ -2829,7 +2829,7 @@
         </is>
       </c>
       <c r="B149" s="1" t="n">
-        <v>0.2306476490784446</v>
+        <v>0.2306476255264149</v>
       </c>
       <c r="C149" s="1" t="n">
         <v>0.1941900998086197</v>
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="B150" s="1" t="n">
-        <v>0.2389747551049</v>
+        <v>0.2389747313935069</v>
       </c>
       <c r="C150" s="1" t="n">
         <v>0.1865178271998318</v>
@@ -2855,7 +2855,7 @@
         </is>
       </c>
       <c r="B151" s="1" t="n">
-        <v>0.2433521334986288</v>
+        <v>0.2433521097034619</v>
       </c>
       <c r="C151" s="1" t="n">
         <v>0.1982380637700829</v>
@@ -2868,7 +2868,7 @@
         </is>
       </c>
       <c r="B152" s="1" t="n">
-        <v>0.2434957051508124</v>
+        <v>0.2434956813528979</v>
       </c>
       <c r="C152" s="1" t="n">
         <v>0.1999979315201648</v>
@@ -2881,7 +2881,7 @@
         </is>
       </c>
       <c r="B153" s="1" t="n">
-        <v>0.2428686339090427</v>
+        <v>0.242868610123129</v>
       </c>
       <c r="C153" s="1" t="n">
         <v>0.196799831865786</v>
@@ -2894,7 +2894,7 @@
         </is>
       </c>
       <c r="B154" s="1" t="n">
-        <v>0.2286255185026238</v>
+        <v>0.2286255111910029</v>
       </c>
       <c r="C154" s="1" t="n">
         <v>0.1802366711213452</v>
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="B155" s="1" t="n">
-        <v>0.2175837580368125</v>
+        <v>0.217583734641978</v>
       </c>
       <c r="C155" s="1" t="n">
         <v>0.1772294589578156</v>
@@ -2920,7 +2920,7 @@
         </is>
       </c>
       <c r="B156" s="1" t="n">
-        <v>0.2108996616812888</v>
+        <v>0.2108996384148836</v>
       </c>
       <c r="C156" s="1" t="n">
         <v>0.1709900555278292</v>
@@ -2933,7 +2933,7 @@
         </is>
       </c>
       <c r="B157" s="1" t="n">
-        <v>0.2127630209616251</v>
+        <v>0.2127629976594172</v>
       </c>
       <c r="C157" s="1" t="n">
         <v>0.1815571784326235</v>
@@ -2946,7 +2946,7 @@
         </is>
       </c>
       <c r="B158" s="1" t="n">
-        <v>0.2060625275217525</v>
+        <v>0.2060625043482889</v>
       </c>
       <c r="C158" s="1" t="n">
         <v>0.1765730358203876</v>
@@ -2959,7 +2959,7 @@
         </is>
       </c>
       <c r="B159" s="1" t="n">
-        <v>0.2074786460427323</v>
+        <v>0.207478639946419</v>
       </c>
       <c r="C159" s="1" t="n">
         <v>0.1682914554481674</v>
@@ -2972,7 +2972,7 @@
         </is>
       </c>
       <c r="B160" s="1" t="n">
-        <v>0.2053931625669774</v>
+        <v>0.2053931392233597</v>
       </c>
       <c r="C160" s="1" t="n">
         <v>0.16858436240737</v>
@@ -2985,7 +2985,7 @@
         </is>
       </c>
       <c r="B161" s="1" t="n">
-        <v>0.2133022255918378</v>
+        <v>0.2133022020950532</v>
       </c>
       <c r="C161" s="1" t="n">
         <v>0.1673343366311746</v>
@@ -2998,7 +2998,7 @@
         </is>
       </c>
       <c r="B162" s="1" t="n">
-        <v>0.2230964904728776</v>
+        <v>0.2230964667864175</v>
       </c>
       <c r="C162" s="1" t="n">
         <v>0.1740470644281025</v>
@@ -3011,7 +3011,7 @@
         </is>
       </c>
       <c r="B163" s="1" t="n">
-        <v>0.2111481705450322</v>
+        <v>0.211148147089963</v>
       </c>
       <c r="C163" s="1" t="n">
         <v>0.1604857531216959</v>
@@ -3024,7 +3024,7 @@
         </is>
       </c>
       <c r="B164" s="1" t="n">
-        <v>0.2130502154669136</v>
+        <v>0.2130501919750094</v>
       </c>
       <c r="C164" s="1" t="n">
         <v>0.1517178246206166</v>
@@ -3037,7 +3037,7 @@
         </is>
       </c>
       <c r="B165" s="1" t="n">
-        <v>0.1999816470253457</v>
+        <v>0.1999816237865271</v>
       </c>
       <c r="C165" s="1" t="n">
         <v>0.1428347252053261</v>
@@ -3050,7 +3050,7 @@
         </is>
       </c>
       <c r="B166" s="1" t="n">
-        <v>0.1994145078995058</v>
+        <v>0.1994144846716703</v>
       </c>
       <c r="C166" s="1" t="n">
         <v>0.1426647778806973</v>
@@ -3063,7 +3063,7 @@
         </is>
       </c>
       <c r="B167" s="1" t="n">
-        <v>0.2050930195732126</v>
+        <v>0.2050929962354073</v>
       </c>
       <c r="C167" s="1" t="n">
         <v>0.1505253843015268</v>
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="B168" s="1" t="n">
-        <v>0.2145558069877458</v>
+        <v>0.2145557834666845</v>
       </c>
       <c r="C168" s="1" t="n">
         <v>0.1473298383259554</v>
@@ -3089,7 +3089,7 @@
         </is>
       </c>
       <c r="B169" s="1" t="n">
-        <v>0.2259554523380858</v>
+        <v>0.2259554285962593</v>
       </c>
       <c r="C169" s="1" t="n">
         <v>0.1600019586716444</v>
@@ -3102,7 +3102,7 @@
         </is>
       </c>
       <c r="B170" s="1" t="n">
-        <v>0.2224531431034975</v>
+        <v>0.2224531194294967</v>
       </c>
       <c r="C170" s="1" t="n">
         <v>0.1443906817026415</v>
@@ -3115,7 +3115,7 @@
         </is>
       </c>
       <c r="B171" s="1" t="n">
-        <v>0.2253821711726314</v>
+        <v>0.2253821474419071</v>
       </c>
       <c r="C171" s="1" t="n">
         <v>0.1520786594360943</v>
@@ -3128,7 +3128,7 @@
         </is>
       </c>
       <c r="B172" s="1" t="n">
-        <v>0.235978934062073</v>
+        <v>0.235978910126132</v>
       </c>
       <c r="C172" s="1" t="n">
         <v>0.1592959941653536</v>
@@ -3141,7 +3141,7 @@
         </is>
       </c>
       <c r="B173" s="1" t="n">
-        <v>0.2470658675986859</v>
+        <v>0.2470658434480355</v>
       </c>
       <c r="C173" s="1" t="n">
         <v>0.1761154165781114</v>
@@ -3154,7 +3154,7 @@
         </is>
       </c>
       <c r="B174" s="1" t="n">
-        <v>0.2494882383268611</v>
+        <v>0.2494882141292991</v>
       </c>
       <c r="C174" s="1" t="n">
         <v>0.1806236811445985</v>
@@ -3167,7 +3167,7 @@
         </is>
       </c>
       <c r="B175" s="1" t="n">
-        <v>0.2607031441589007</v>
+        <v>0.2607031197441512</v>
       </c>
       <c r="C175" s="1" t="n">
         <v>0.1787383000811356</v>
@@ -3180,7 +3180,7 @@
         </is>
       </c>
       <c r="B176" s="1" t="n">
-        <v>0.258210965064553</v>
+        <v>0.258210940698067</v>
       </c>
       <c r="C176" s="1" t="n">
         <v>0.1808590026466954</v>
@@ -3193,7 +3193,7 @@
         </is>
       </c>
       <c r="B177" s="1" t="n">
-        <v>0.2592843603805826</v>
+        <v>0.2592843359933092</v>
       </c>
       <c r="C177" s="1" t="n">
         <v>0.1808590026466954</v>
@@ -3206,7 +3206,7 @@
         </is>
       </c>
       <c r="B178" s="1" t="n">
-        <v>0.2549084392413177</v>
+        <v>0.2549084149387884</v>
       </c>
       <c r="C178" s="1" t="n">
         <v>0.1759062702837899</v>
@@ -3219,7 +3219,7 @@
         </is>
       </c>
       <c r="B179" s="1" t="n">
-        <v>0.2446898664123105</v>
+        <v>0.2446898423076738</v>
       </c>
       <c r="C179" s="1" t="n">
         <v>0.16770832289251</v>
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="B180" s="1" t="n">
-        <v>0.2395406645244811</v>
+        <v>0.2395406405195637</v>
       </c>
       <c r="C180" s="1" t="n">
         <v>0.1639585009318043</v>
@@ -3245,7 +3245,7 @@
         </is>
       </c>
       <c r="B181" s="1" t="n">
-        <v>0.2373376992089695</v>
+        <v>0.2373376752467147</v>
       </c>
       <c r="C181" s="1" t="n">
         <v>0.1656190305762804</v>
@@ -3258,7 +3258,7 @@
         </is>
       </c>
       <c r="B182" s="1" t="n">
-        <v>0.2450398497061761</v>
+        <v>0.2450398255947615</v>
       </c>
       <c r="C182" s="1" t="n">
         <v>0.1734560154681419</v>
@@ -3271,7 +3271,7 @@
         </is>
       </c>
       <c r="B183" s="1" t="n">
-        <v>0.2392867648885213</v>
+        <v>0.2392867408885209</v>
       </c>
       <c r="C183" s="1" t="n">
         <v>0.1667721442417371</v>
@@ -3284,7 +3284,7 @@
         </is>
       </c>
       <c r="B184" s="1" t="n">
-        <v>0.2361114759284662</v>
+        <v>0.2361114519899583</v>
       </c>
       <c r="C184" s="1" t="n">
         <v>0.1682208462291439</v>
@@ -3297,7 +3297,7 @@
         </is>
       </c>
       <c r="B185" s="1" t="n">
-        <v>0.2480753052665778</v>
+        <v>0.2480752810963789</v>
       </c>
       <c r="C185" s="1" t="n">
         <v>0.1780688531817898</v>
@@ -3310,7 +3310,7 @@
         </is>
       </c>
       <c r="B186" s="1" t="n">
-        <v>0.2464589375056632</v>
+        <v>0.2464589133667667</v>
       </c>
       <c r="C186" s="1" t="n">
         <v>0.1637439919119872</v>
@@ -3323,7 +3323,7 @@
         </is>
       </c>
       <c r="B187" s="1" t="n">
-        <v>0.2509667482933298</v>
+        <v>0.2509667240671352</v>
       </c>
       <c r="C187" s="1" t="n">
         <v>0.1645833861359616</v>
@@ -3336,7 +3336,7 @@
         </is>
       </c>
       <c r="B188" s="1" t="n">
-        <v>0.249162801313741</v>
+        <v>0.2491627771224816</v>
       </c>
       <c r="C188" s="1" t="n">
         <v>0.1620783549098963</v>
@@ -3349,7 +3349,7 @@
         </is>
       </c>
       <c r="B189" s="1" t="n">
-        <v>0.2487867964593828</v>
+        <v>0.2487867722754051</v>
       </c>
       <c r="C189" s="1" t="n">
         <v>0.1511608672727343</v>
@@ -3362,7 +3362,7 @@
         </is>
       </c>
       <c r="B190" s="1" t="n">
-        <v>0.2424780422189043</v>
+        <v>0.2424780181571018</v>
       </c>
       <c r="C190" s="1" t="n">
         <v>0.1322807537463893</v>
@@ -3375,7 +3375,7 @@
         </is>
       </c>
       <c r="B191" s="1" t="n">
-        <v>0.2342169700301922</v>
+        <v>0.2342169461283734</v>
       </c>
       <c r="C191" s="1" t="n">
         <v>0.129681491772333</v>
@@ -3388,7 +3388,7 @@
         </is>
       </c>
       <c r="B192" s="1" t="n">
-        <v>0.2390437882859884</v>
+        <v>0.2390437642906935</v>
       </c>
       <c r="C192" s="1" t="n">
         <v>0.1342262739457651</v>
@@ -3401,7 +3401,7 @@
         </is>
       </c>
       <c r="B193" s="1" t="n">
-        <v>0.225438999947899</v>
+        <v>0.2254389762160742</v>
       </c>
       <c r="C193" s="1" t="n">
         <v>0.1175139783589754</v>
@@ -3414,7 +3414,7 @@
         </is>
       </c>
       <c r="B194" s="1" t="n">
-        <v>0.2163200511339798</v>
+        <v>0.2163200275787525</v>
       </c>
       <c r="C194" s="1" t="n">
         <v>0.1177702400272924</v>
@@ -3427,7 +3427,7 @@
         </is>
       </c>
       <c r="B195" s="1" t="n">
-        <v>0.2236004069091255</v>
+        <v>0.223600383212907</v>
       </c>
       <c r="C195" s="1" t="n">
         <v>0.1243574545108392</v>
@@ -3440,7 +3440,7 @@
         </is>
       </c>
       <c r="B196" s="1" t="n">
-        <v>0.2272233513483592</v>
+        <v>0.2272233275819788</v>
       </c>
       <c r="C196" s="1" t="n">
         <v>0.1213109156936765</v>
@@ -3453,7 +3453,7 @@
         </is>
       </c>
       <c r="B197" s="1" t="n">
-        <v>0.2296566786831042</v>
+        <v>0.2296566548696</v>
       </c>
       <c r="C197" s="1" t="n">
         <v>0.1213999114001123</v>
@@ -3466,7 +3466,7 @@
         </is>
       </c>
       <c r="B198" s="1" t="n">
-        <v>0.2134421882451716</v>
+        <v>0.2134421647456768</v>
       </c>
       <c r="C198" s="1" t="n">
         <v>0.1059873106423208</v>
@@ -3479,7 +3479,7 @@
         </is>
       </c>
       <c r="B199" s="1" t="n">
-        <v>0.2192686597670093</v>
+        <v>0.2192686361546792</v>
       </c>
       <c r="C199" s="1" t="n">
         <v>0.1149565967173591</v>
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="B200" s="1" t="n">
-        <v>0.2203727064270118</v>
+        <v>0.2203726827933008</v>
       </c>
       <c r="C200" s="1" t="n">
         <v>0.1135026596883972</v>
@@ -3505,7 +3505,7 @@
         </is>
       </c>
       <c r="B201" s="1" t="n">
-        <v>0.2327430664022352</v>
+        <v>0.2327430425289601</v>
       </c>
       <c r="C201" s="1" t="n">
         <v>0.1266585744841378</v>
@@ -3518,7 +3518,7 @@
         </is>
       </c>
       <c r="B202" s="1" t="n">
-        <v>0.2319487330491516</v>
+        <v>0.2319487091912598</v>
       </c>
       <c r="C202" s="1" t="n">
         <v>0.1337608659831262</v>
@@ -3531,7 +3531,7 @@
         </is>
       </c>
       <c r="B203" s="1" t="n">
-        <v>0.2440446282034139</v>
+        <v>0.2440446041112732</v>
       </c>
       <c r="C203" s="1" t="n">
         <v>0.1396654821214696</v>
@@ -3544,7 +3544,7 @@
         </is>
       </c>
       <c r="B204" s="1" t="n">
-        <v>0.2565743526666013</v>
+        <v>0.2565743283318103</v>
       </c>
       <c r="C204" s="1" t="n">
         <v>0.1445580753484621</v>
@@ -3557,7 +3557,7 @@
         </is>
       </c>
       <c r="B205" s="1" t="n">
-        <v>0.2512947046675724</v>
+        <v>0.2512946804350269</v>
       </c>
       <c r="C205" s="1" t="n">
         <v>0.1374086684754783</v>
@@ -3570,7 +3570,7 @@
         </is>
       </c>
       <c r="B206" s="1" t="n">
-        <v>0.2345550384502237</v>
+        <v>0.2345550145418582</v>
       </c>
       <c r="C206" s="1" t="n">
         <v>0.131700174869539</v>
@@ -3583,7 +3583,7 @@
         </is>
       </c>
       <c r="B207" s="1" t="n">
-        <v>0.2385784621226901</v>
+        <v>0.2385784381364071</v>
       </c>
       <c r="C207" s="1" t="n">
         <v>0.1436898245539648</v>
@@ -3596,7 +3596,7 @@
         </is>
       </c>
       <c r="B208" s="1" t="n">
-        <v>0.237509805811666</v>
+        <v>0.2375097818460785</v>
       </c>
       <c r="C208" s="1" t="n">
         <v>0.1435774626864417</v>
@@ -3609,7 +3609,7 @@
         </is>
       </c>
       <c r="B209" s="1" t="n">
-        <v>0.214925276621899</v>
+        <v>0.2149252530936829</v>
       </c>
       <c r="C209" s="1" t="n">
         <v>0.1282537299511459</v>
@@ -3622,7 +3622,7 @@
         </is>
       </c>
       <c r="B210" s="1" t="n">
-        <v>0.1979306307182742</v>
+        <v>0.197930607519176</v>
       </c>
       <c r="C210" s="1" t="n">
         <v>0.1186829248330374</v>
@@ -3635,7 +3635,7 @@
         </is>
       </c>
       <c r="B211" s="1" t="n">
-        <v>0.1814962524533117</v>
+        <v>0.1814962295724813</v>
       </c>
       <c r="C211" s="1" t="n">
         <v>0.1046039828323821</v>
@@ -3648,7 +3648,7 @@
         </is>
       </c>
       <c r="B212" s="1" t="n">
-        <v>0.1845197997707237</v>
+        <v>0.1845197768313394</v>
       </c>
       <c r="C212" s="1" t="n">
         <v>0.1027420956139469</v>
@@ -3661,7 +3661,7 @@
         </is>
       </c>
       <c r="B213" s="1" t="n">
-        <v>0.1856383403315689</v>
+        <v>0.1856383173705229</v>
       </c>
       <c r="C213" s="1" t="n">
         <v>0.1107543905559327</v>
@@ -3674,7 +3674,7 @@
         </is>
       </c>
       <c r="B214" s="1" t="n">
-        <v>0.1952159179533461</v>
+        <v>0.1952158948068212</v>
       </c>
       <c r="C214" s="1" t="n">
         <v>0.09482658509875952</v>
@@ -3687,7 +3687,7 @@
         </is>
       </c>
       <c r="B215" s="1" t="n">
-        <v>0.1813234110059425</v>
+        <v>0.1813233881284595</v>
       </c>
       <c r="C215" s="1" t="n">
         <v>0.08187202787697823</v>
@@ -3700,7 +3700,7 @@
         </is>
       </c>
       <c r="B216" s="1" t="n">
-        <v>0.1775656495814002</v>
+        <v>0.1775656267766899</v>
       </c>
       <c r="C216" s="1" t="n">
         <v>0.07667873897042088</v>
@@ -3713,7 +3713,7 @@
         </is>
       </c>
       <c r="B217" s="1" t="n">
-        <v>0.1872316957964371</v>
+        <v>0.1872316728045342</v>
       </c>
       <c r="C217" s="1" t="n">
         <v>0.08960967466323422</v>
@@ -3726,7 +3726,7 @@
         </is>
       </c>
       <c r="B218" s="1" t="n">
-        <v>0.1917768345293909</v>
+        <v>0.1917768114494669</v>
       </c>
       <c r="C218" s="1" t="n">
         <v>0.09666485078822706</v>
@@ -3739,7 +3739,7 @@
         </is>
       </c>
       <c r="B219" s="1" t="n">
-        <v>0.209616817851408</v>
+        <v>0.2096167944259952</v>
       </c>
       <c r="C219" s="1" t="n">
         <v>0.1081864111472668</v>
@@ -3752,7 +3752,7 @@
         </is>
       </c>
       <c r="B220" s="1" t="n">
-        <v>0.2210069811757738</v>
+        <v>0.2210069575297793</v>
       </c>
       <c r="C220" s="1" t="n">
         <v>0.1290852077708182</v>
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="B221" s="1" t="n">
-        <v>0.2193269558040654</v>
+        <v>0.2193269321906062</v>
       </c>
       <c r="C221" s="1" t="n">
         <v>0.1396915296453052</v>
@@ -3778,7 +3778,7 @@
         </is>
       </c>
       <c r="B222" s="1" t="n">
-        <v>0.2257622197477822</v>
+        <v>0.2257621960096978</v>
       </c>
       <c r="C222" s="1" t="n">
         <v>0.1416894002602316</v>
@@ -3791,7 +3791,7 @@
         </is>
       </c>
       <c r="B223" s="1" t="n">
-        <v>0.2336243852372006</v>
+        <v>0.2336243613468578</v>
       </c>
       <c r="C223" s="1" t="n">
         <v>0.1449319339258581</v>
@@ -3804,7 +3804,7 @@
         </is>
       </c>
       <c r="B224" s="1" t="n">
-        <v>0.2393671155525423</v>
+        <v>0.2393670915509858</v>
       </c>
       <c r="C224" s="1" t="n">
         <v>0.1460824939125074</v>
@@ -3817,7 +3817,7 @@
         </is>
       </c>
       <c r="B225" s="1" t="n">
-        <v>0.2448406695468177</v>
+        <v>0.2448406454392604</v>
       </c>
       <c r="C225" s="1" t="n">
         <v>0.1368177471994592</v>
@@ -3830,7 +3830,7 @@
         </is>
       </c>
       <c r="B226" s="1" t="n">
-        <v>0.2481449345753624</v>
+        <v>0.2481449104038147</v>
       </c>
       <c r="C226" s="1" t="n">
         <v>0.1545707945841823</v>
@@ -3843,7 +3843,7 @@
         </is>
       </c>
       <c r="B227" s="1" t="n">
-        <v>0.2466644759769716</v>
+        <v>0.2466644518340944</v>
       </c>
       <c r="C227" s="1" t="n">
         <v>0.1536057593628866</v>
@@ -3856,7 +3856,7 @@
         </is>
       </c>
       <c r="B228" s="1" t="n">
-        <v>0.2598977525690469</v>
+        <v>0.2598977281698942</v>
       </c>
       <c r="C228" s="1" t="n">
         <v>0.1756108096457798</v>
@@ -3869,7 +3869,7 @@
         </is>
       </c>
       <c r="B229" s="1" t="n">
-        <v>0.2646590249334642</v>
+        <v>0.2646590004421048</v>
       </c>
       <c r="C229" s="1" t="n">
         <v>0.17748827430494</v>
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="B230" s="1" t="n">
-        <v>0.2664926084752015</v>
+        <v>0.266492583948333</v>
       </c>
       <c r="C230" s="1" t="n">
         <v>0.1788899886022917</v>
@@ -3895,7 +3895,7 @@
         </is>
       </c>
       <c r="B231" s="1" t="n">
-        <v>0.2733255946708097</v>
+        <v>0.2733255700116137</v>
       </c>
       <c r="C231" s="1" t="n">
         <v>0.1804013834044187</v>
@@ -3908,7 +3908,7 @@
         </is>
       </c>
       <c r="B232" s="1" t="n">
-        <v>0.2789160436289768</v>
+        <v>0.2789160188615163</v>
       </c>
       <c r="C232" s="1" t="n">
         <v>0.1891248778942503</v>
@@ -3921,7 +3921,7 @@
         </is>
       </c>
       <c r="B233" s="1" t="n">
-        <v>0.2786312496055281</v>
+        <v>0.2786312248435827</v>
       </c>
       <c r="C233" s="1" t="n">
         <v>0.1867217384525981</v>
@@ -3934,7 +3934,7 @@
         </is>
       </c>
       <c r="B234" s="1" t="n">
-        <v>0.2884557073931437</v>
+        <v>0.2884556824409381</v>
       </c>
       <c r="C234" s="1" t="n">
         <v>0.1915411687817603</v>
@@ -3947,7 +3947,7 @@
         </is>
       </c>
       <c r="B235" s="1" t="n">
-        <v>0.2896513685147346</v>
+        <v>0.2896513435393739</v>
       </c>
       <c r="C235" s="1" t="n">
         <v>0.1915411687817603</v>
@@ -3960,7 +3960,7 @@
         </is>
       </c>
       <c r="B236" s="1" t="n">
-        <v>0.2918149528297818</v>
+        <v>0.2918149278125211</v>
       </c>
       <c r="C236" s="1" t="n">
         <v>0.192252368329606</v>
@@ -3973,7 +3973,7 @@
         </is>
       </c>
       <c r="B237" s="1" t="n">
-        <v>0.2854078030048315</v>
+        <v>0.2854077781116515</v>
       </c>
       <c r="C237" s="1" t="n">
         <v>0.1899225194697247</v>
@@ -3986,7 +3986,7 @@
         </is>
       </c>
       <c r="B238" s="1" t="n">
-        <v>0.2866441566022409</v>
+        <v>0.2866441316851176</v>
       </c>
       <c r="C238" s="1" t="n">
         <v>0.1910887845810392</v>
@@ -3999,7 +3999,7 @@
         </is>
       </c>
       <c r="B239" s="1" t="n">
-        <v>0.2894372609311349</v>
+        <v>0.2894372359599204</v>
       </c>
       <c r="C239" s="1" t="n">
         <v>0.1899617184394173</v>
@@ -4012,7 +4012,7 @@
         </is>
       </c>
       <c r="B240" s="1" t="n">
-        <v>0.3017883345588357</v>
+        <v>0.3017883093484308</v>
       </c>
       <c r="C240" s="1" t="n">
         <v>0.194464620280409</v>
@@ -4025,7 +4025,7 @@
         </is>
       </c>
       <c r="B241" s="1" t="n">
-        <v>0.3017883345588357</v>
+        <v>0.3017883093484308</v>
       </c>
       <c r="C241" s="1" t="n">
         <v>0.194464620280409</v>
@@ -4159,13 +4159,13 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.01031434507052587</v>
+        <v>0.01031428309586024</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0.03375085031185554</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>-0.04374322677499454</v>
+        <v>-0.04374322396429664</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>0.01726045181352398</v>
@@ -4184,13 +4184,13 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>-0.01060472982777738</v>
+        <v>-0.01060460839632893</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0.0006732342514317313</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>-0.02963775111395472</v>
+        <v>-0.02963781631622664</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>-0.002888076797592731</v>
@@ -4209,13 +4209,13 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.03679412570411911</v>
+        <v>0.0367941211882663</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.009418080144487861</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.01178539985920901</v>
+        <v>0.01178533061316411</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>0.005611780984804415</v>
@@ -4234,13 +4234,13 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0.004088873968074669</v>
+        <v>0.004088755106652631</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0.01432856331507937</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0.009736265809001665</v>
+        <v>0.009736403354272838</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>0.004680566980618694</v>
@@ -4265,7 +4265,7 @@
         <v>-0.006570309520439799</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.00761720014247258</v>
+        <v>0.007617131846648029</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>-0.002150267670138928</v>
@@ -4309,7 +4309,7 @@
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>-0.0005993259135237405</v>
+        <v>-0.0005994408590384026</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0.008737851559167842</v>
@@ -4334,13 +4334,13 @@
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.01011908595719624</v>
+        <v>0.01011920213549655</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>-0.006737251777299891</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.003018728366081191</v>
+        <v>0.003018792908818568</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>0.003345661085441876</v>
@@ -4384,13 +4384,13 @@
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.008756235809203705</v>
+        <v>0.008756349671467545</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.01315368503983905</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.004681802846403738</v>
+        <v>0.004681738196654406</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>-0.005035634587212789</v>
@@ -4409,7 +4409,7 @@
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>-0.005369976419510758</v>
+        <v>-0.005369975813380612</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>-0.005383169206004901</v>
@@ -4434,7 +4434,7 @@
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.0004438332485234842</v>
+        <v>0.0004438331981557742</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>-0.02324099164597015</v>
@@ -4459,7 +4459,7 @@
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.01922076313392163</v>
+        <v>0.01922064752069574</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.01271188175538818</v>
@@ -4484,13 +4484,13 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.02350046882521029</v>
+        <v>0.0235003575313919</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.01609267996954955</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>0.009824288116401902</v>
+        <v>0.009824352199687691</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>0.01017494261084195</v>
@@ -4509,13 +4509,13 @@
         </is>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.01006297911504772</v>
+        <v>0.01006308894770669</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>-0.0009502609720638544</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>-0.002226044196731114</v>
+        <v>-0.002226107515300613</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>-0.005478046040928386</v>
@@ -4559,7 +4559,7 @@
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>0.01480336951043015</v>
+        <v>0.01480347767396473</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.01337154655965356</v>
@@ -4584,13 +4584,13 @@
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>0.01368432575107481</v>
+        <v>0.0136841111211301</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0.003141724576239291</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>0.0006451239664702069</v>
+        <v>0.0006451860394005582</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>-0.002367920389281686</v>
@@ -4609,13 +4609,13 @@
         </is>
       </c>
       <c r="B22" s="1" t="n">
-        <v>-0.02007800003133375</v>
+        <v>-0.02007789699561791</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0.003131823587420035</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>-0.02196157371293339</v>
+        <v>-0.02196163438350085</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>0.01497165814838963</v>
@@ -4659,7 +4659,7 @@
         </is>
       </c>
       <c r="B24" s="1" t="n">
-        <v>0.007900781262378809</v>
+        <v>0.007900674920432227</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>0.006929135279573284</v>
@@ -4684,7 +4684,7 @@
         </is>
       </c>
       <c r="B25" s="1" t="n">
-        <v>0.03706255051871588</v>
+        <v>0.03706265993748414</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>-0.02783860156670293</v>
@@ -4759,7 +4759,7 @@
         </is>
       </c>
       <c r="B28" s="1" t="n">
-        <v>0.01924466843066774</v>
+        <v>0.01924476955818899</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>-0.0108177204241986</v>
@@ -4784,7 +4784,7 @@
         </is>
       </c>
       <c r="B29" s="1" t="n">
-        <v>-0.01765268624081062</v>
+        <v>-0.01765278370743684</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>-0.01254418028529791</v>
@@ -4834,13 +4834,13 @@
         </is>
       </c>
       <c r="B31" s="1" t="n">
-        <v>0.002456252796223746</v>
+        <v>0.002456151092244729</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>-0.008018015970818748</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>-0.001972232710612976</v>
+        <v>-0.001972349500611759</v>
       </c>
       <c r="E31" s="1" t="n">
         <v>0.004403690887457401</v>
@@ -4859,13 +4859,13 @@
         </is>
       </c>
       <c r="B32" s="1" t="n">
-        <v>0.01880677409510456</v>
+        <v>0.01880687745793264</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0.0109925952022758</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>0.03124279590754897</v>
+        <v>0.03124291658441081</v>
       </c>
       <c r="E32" s="1" t="n">
         <v>0.01351844999651441</v>
@@ -4909,7 +4909,7 @@
         </is>
       </c>
       <c r="B34" s="1" t="n">
-        <v>0.01390332286886453</v>
+        <v>0.01390342287334478</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>0.02057217345145324</v>
@@ -4934,7 +4934,7 @@
         </is>
       </c>
       <c r="B35" s="1" t="n">
-        <v>-0.01042927218893297</v>
+        <v>-0.01042936979340303</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>-0.007244093164233245</v>
@@ -5059,7 +5059,7 @@
         </is>
       </c>
       <c r="B40" s="1" t="n">
-        <v>0.003290588164726715</v>
+        <v>0.003290485279188626</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>0.006732868328391151</v>
@@ -5084,7 +5084,7 @@
         </is>
       </c>
       <c r="B41" s="1" t="n">
-        <v>-0.01800529189187083</v>
+        <v>-0.01800529373827942</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>-0.01019105676497567</v>
@@ -5109,7 +5109,7 @@
         </is>
       </c>
       <c r="B42" s="1" t="n">
-        <v>0.008247333970137438</v>
+        <v>0.008247543688130188</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>0.008687246130473003</v>
@@ -5134,7 +5134,7 @@
         </is>
       </c>
       <c r="B43" s="1" t="n">
-        <v>-0.003447776206097597</v>
+        <v>-0.003447775848997248</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>-0.00223283543367403</v>
@@ -5159,13 +5159,13 @@
         </is>
       </c>
       <c r="B44" s="1" t="n">
-        <v>-0.01424602543996956</v>
+        <v>-0.01424602395934493</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>0.00607411582100581</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>-0.01262920563598657</v>
+        <v>-0.01262926720132473</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>-0.004524908581630571</v>
@@ -5184,13 +5184,13 @@
         </is>
       </c>
       <c r="B45" s="1" t="n">
-        <v>0.004129236977863382</v>
+        <v>0.004129131108004724</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>0.01965316751311641</v>
+        <v>0.01965323109135486</v>
       </c>
       <c r="E45" s="1" t="n">
         <v>0.02026513487839066</v>
@@ -5209,13 +5209,13 @@
         </is>
       </c>
       <c r="B46" s="1" t="n">
-        <v>0.03509005142420629</v>
+        <v>0.03509015642513824</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>0.007944067220718942</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>0.01664603432136214</v>
+        <v>0.01664609547235596</v>
       </c>
       <c r="E46" s="1" t="n">
         <v>-0.001670651362219555</v>
@@ -5234,13 +5234,13 @@
         </is>
       </c>
       <c r="B47" s="1" t="n">
-        <v>0.01853942107218831</v>
+        <v>0.01853931775018536</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>0.005674665934060519</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>0.00618910741155454</v>
+        <v>0.006189046889545802</v>
       </c>
       <c r="E47" s="1" t="n">
         <v>-0.02380066227575417</v>
@@ -5290,7 +5290,7 @@
         <v>0.004727346099755447</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>-0.001770534306941962</v>
+        <v>-0.001770594726485553</v>
       </c>
       <c r="E49" s="1" t="n">
         <v>0.001331005141085528</v>
@@ -5315,7 +5315,7 @@
         <v>0.01035128914909267</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>-0.005439474744383554</v>
+        <v>-0.005439414546905219</v>
       </c>
       <c r="E50" s="1" t="n">
         <v>0.003228324884762213</v>
@@ -5359,7 +5359,7 @@
         </is>
       </c>
       <c r="B52" s="1" t="n">
-        <v>0.01326596082835696</v>
+        <v>0.01326606399796471</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>-0.02970616283862604</v>
@@ -5384,13 +5384,13 @@
         </is>
       </c>
       <c r="B53" s="1" t="n">
-        <v>0.01408928966158562</v>
+        <v>0.01408918640815804</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>0.02529115760784939</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>0.0270558846934732</v>
+        <v>0.02705576374493912</v>
       </c>
       <c r="E53" s="1" t="n">
         <v>0.003746727140466088</v>
@@ -5409,13 +5409,13 @@
         </is>
       </c>
       <c r="B54" s="1" t="n">
-        <v>0.002621354359055861</v>
+        <v>0.002621454763313436</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>-0.04868545214940845</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>0.0178304002848908</v>
+        <v>0.01783040238464118</v>
       </c>
       <c r="E54" s="1" t="n">
         <v>0.0007464898758908767</v>
@@ -5434,13 +5434,13 @@
         </is>
       </c>
       <c r="B55" s="1" t="n">
-        <v>0.0186940614439739</v>
+        <v>0.01869395943017738</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>0.02661211397806618</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>0.04053632689338893</v>
+        <v>0.04053656298224961</v>
       </c>
       <c r="E55" s="1" t="n">
         <v>0.02331217776024608</v>
@@ -5465,7 +5465,7 @@
         <v>-0.01395813407732538</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>0.01169440501449603</v>
+        <v>0.01169440371417108</v>
       </c>
       <c r="E56" s="1" t="n">
         <v>-0.00364498467043517</v>
@@ -5490,7 +5490,7 @@
         <v>0.0144927593754236</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>-0.02576665755539387</v>
+        <v>-0.02576676463024064</v>
       </c>
       <c r="E57" s="1" t="n">
         <v>-0.003292408516962886</v>
@@ -5509,7 +5509,7 @@
         </is>
       </c>
       <c r="B58" s="1" t="n">
-        <v>0.01194410071317109</v>
+        <v>0.01194400337716983</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>0.0182723960040907</v>
@@ -5534,7 +5534,7 @@
         </is>
       </c>
       <c r="B59" s="1" t="n">
-        <v>-0.009103438776553507</v>
+        <v>-0.009103343465045599</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>0.008482861285229237</v>
@@ -5559,7 +5559,7 @@
         </is>
       </c>
       <c r="B60" s="1" t="n">
-        <v>0.006969490061793371</v>
+        <v>0.006969392990982648</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>-0.004852756232196276</v>
@@ -5584,7 +5584,7 @@
         </is>
       </c>
       <c r="B61" s="1" t="n">
-        <v>0.00830554151344054</v>
+        <v>0.008305735112022816</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>-0.03153443990588012</v>
@@ -5609,7 +5609,7 @@
         </is>
       </c>
       <c r="B62" s="1" t="n">
-        <v>-0.01229326155571753</v>
+        <v>-0.01229335598532078</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>0.01658029463166044</v>
@@ -5634,7 +5634,7 @@
         </is>
       </c>
       <c r="B63" s="1" t="n">
-        <v>-0.003980300315648</v>
+        <v>-0.003980397110480705</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>0.01087324809738255</v>
@@ -5659,13 +5659,13 @@
         </is>
       </c>
       <c r="B64" s="1" t="n">
-        <v>0.01979075042597134</v>
+        <v>0.01979084953092358</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>0.01109243441028762</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>0.01918395762131153</v>
+        <v>0.01918384603736967</v>
       </c>
       <c r="E64" s="1" t="n">
         <v>0.0157808593255806</v>
@@ -5684,13 +5684,13 @@
         </is>
       </c>
       <c r="B65" s="1" t="n">
-        <v>0.009889784837620041</v>
+        <v>0.009889880133292062</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>0.02460105628308096</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>0.01261973812176698</v>
+        <v>0.0126198489870466</v>
       </c>
       <c r="E65" s="1" t="n">
         <v>-0.01125002778224704</v>
@@ -5709,13 +5709,13 @@
         </is>
       </c>
       <c r="B66" s="1" t="n">
-        <v>0.01564425583697782</v>
+        <v>0.01564415999830904</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>0.01784559214325832</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>0.01496207233324309</v>
+        <v>0.01496218045242048</v>
       </c>
       <c r="E66" s="1" t="n">
         <v>0.006501711772948893</v>
@@ -5734,13 +5734,13 @@
         </is>
       </c>
       <c r="B67" s="1" t="n">
-        <v>0.007701780832417793</v>
+        <v>0.007701687923461709</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>0.00031872238653885</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>-0.003711342754008085</v>
+        <v>-0.003711448883982116</v>
       </c>
       <c r="E67" s="1" t="n">
         <v>0.0057420213651318</v>
@@ -5759,7 +5759,7 @@
         </is>
       </c>
       <c r="B68" s="1" t="n">
-        <v>-0.003249825444506804</v>
+        <v>-0.003249641346398491</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>-0.01306564239570529</v>
@@ -5784,7 +5784,7 @@
         </is>
       </c>
       <c r="B69" s="1" t="n">
-        <v>-0.01129020755308108</v>
+        <v>-0.01129029900820233</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>-0.02970617038074119</v>
@@ -5859,7 +5859,7 @@
         </is>
       </c>
       <c r="B72" s="1" t="n">
-        <v>-0.01597227501197718</v>
+        <v>-0.01597236805634317</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>0</v>
@@ -5884,13 +5884,13 @@
         </is>
       </c>
       <c r="B73" s="1" t="n">
-        <v>-0.007591222986454649</v>
+        <v>-0.007591129149612574</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>0.02644790713032297</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>-0.02266853063022534</v>
+        <v>-0.02266842450613293</v>
       </c>
       <c r="E73" s="1" t="n">
         <v>-0.002638113956059951</v>
@@ -5915,7 +5915,7 @@
         <v>0.01272013671198224</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>0.002333721020004953</v>
+        <v>0.002333612181040889</v>
       </c>
       <c r="E74" s="1" t="n">
         <v>-0.004232009181523333</v>
@@ -5965,7 +5965,7 @@
         <v>0.02172503479179544</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>-0.01276555660490619</v>
+        <v>-0.01276566256423917</v>
       </c>
       <c r="E76" s="1" t="n">
         <v>0.01218417220375256</v>
@@ -5990,7 +5990,7 @@
         <v>0.005395115044719123</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>0.009296125932652721</v>
+        <v>0.009296126930400828</v>
       </c>
       <c r="E77" s="1" t="n">
         <v>0.005487673952502048</v>
@@ -6009,13 +6009,13 @@
         </is>
       </c>
       <c r="B78" s="1" t="n">
-        <v>0.007504660509524363</v>
+        <v>0.007504753232916883</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>0.00536616397273737</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>-0.001488985210108318</v>
+        <v>-0.001488879027542134</v>
       </c>
       <c r="E78" s="1" t="n">
         <v>0.00352113209851046</v>
@@ -6034,13 +6034,13 @@
         </is>
       </c>
       <c r="B79" s="1" t="n">
-        <v>0.006968349303924315</v>
+        <v>0.006968256629898306</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>-0.008477251319618739</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>0.0002775376214705361</v>
+        <v>0.0002774311219995163</v>
       </c>
       <c r="E79" s="1" t="n">
         <v>0.002631565756218368</v>
@@ -6059,13 +6059,13 @@
         </is>
       </c>
       <c r="B80" s="1" t="n">
-        <v>-0.005846409107705175</v>
+        <v>-0.005846317711864946</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>-0.001583256402195699</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>-0.008112475676946396</v>
+        <v>-0.008112476540681146</v>
       </c>
       <c r="E80" s="1" t="n">
         <v>0.003849463038669176</v>
@@ -6084,13 +6084,13 @@
         </is>
       </c>
       <c r="B81" s="1" t="n">
-        <v>-0.009780877851047642</v>
+        <v>-0.009780876951859141</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>0.00126860156383235</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>-0.001223147511160483</v>
+        <v>-0.001223040301721934</v>
       </c>
       <c r="E81" s="1" t="n">
         <v>0.0135960389487455</v>
@@ -6109,13 +6109,13 @@
         </is>
       </c>
       <c r="B82" s="1" t="n">
-        <v>0.001878552691852553</v>
+        <v>0.001878459676063482</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>0.003167576257091964</v>
       </c>
       <c r="D82" s="1" t="n">
-        <v>-0.01396299990950844</v>
+        <v>-0.01396289243733351</v>
       </c>
       <c r="E82" s="1" t="n">
         <v>0.01155710179139646</v>
@@ -6140,7 +6140,7 @@
         <v>0.03504890117868364</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>-0.02253593861105818</v>
+        <v>-0.022535936154775</v>
       </c>
       <c r="E83" s="1" t="n">
         <v>0.007500374616168148</v>
@@ -6165,7 +6165,7 @@
         <v>-0.02623547086725597</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>0.07243470681304265</v>
+        <v>0.07243458722910767</v>
       </c>
       <c r="E84" s="1" t="n">
         <v>-0.00415508778988416</v>
@@ -6190,7 +6190,7 @@
         <v>0.01033834344979012</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>0.03202768826928248</v>
+        <v>0.03202758429374675</v>
       </c>
       <c r="E85" s="1" t="n">
         <v>-0.01164815678564801</v>
@@ -6209,13 +6209,13 @@
         </is>
       </c>
       <c r="B86" s="1" t="n">
-        <v>0.007540986768225899</v>
+        <v>0.007541077740766067</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>-0.004031040871790181</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>0.007971747622681269</v>
+        <v>0.007971849174620571</v>
       </c>
       <c r="E86" s="1" t="n">
         <v>0.007211958811199404</v>
@@ -6234,7 +6234,7 @@
         </is>
       </c>
       <c r="B87" s="1" t="n">
-        <v>-0.0005303731636596698</v>
+        <v>-0.0005303731157714209</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>0</v>
@@ -6259,7 +6259,7 @@
         </is>
       </c>
       <c r="B88" s="1" t="n">
-        <v>-0.006191422131766267</v>
+        <v>-0.006191511911993408</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>-0.00591527500084621</v>
@@ -6334,13 +6334,13 @@
         </is>
       </c>
       <c r="B91" s="1" t="n">
-        <v>0.04692700961694496</v>
+        <v>0.0469269172067428</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>0.009769977238050842</v>
       </c>
       <c r="D91" s="1" t="n">
-        <v>0.01715731500720552</v>
+        <v>0.01715741556466588</v>
       </c>
       <c r="E91" s="1" t="n">
         <v>0.007439451744837955</v>
@@ -6359,13 +6359,13 @@
         </is>
       </c>
       <c r="B92" s="1" t="n">
-        <v>-0.0004032967056246672</v>
+        <v>-0.0004032967412228583</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>0.005617986892395788</v>
       </c>
       <c r="D92" s="1" t="n">
-        <v>-0.006438043397130166</v>
+        <v>-0.006438240483170543</v>
       </c>
       <c r="E92" s="1" t="n">
         <v>-0.000686946863159954</v>
@@ -6384,13 +6384,13 @@
         </is>
       </c>
       <c r="B93" s="1" t="n">
-        <v>-0.009971249211558675</v>
+        <v>-0.009971161788389415</v>
       </c>
       <c r="C93" s="1" t="n">
         <v>0.009621277059249644</v>
       </c>
       <c r="D93" s="1" t="n">
-        <v>-0.005345837135548259</v>
+        <v>-0.0053458376674691</v>
       </c>
       <c r="E93" s="1" t="n">
         <v>0.0003437095417715419</v>
@@ -6415,7 +6415,7 @@
         <v>0.002151850521087795</v>
       </c>
       <c r="D94" s="1" t="n">
-        <v>0.0172963356477478</v>
+        <v>0.01729643741466869</v>
       </c>
       <c r="E94" s="1" t="n">
         <v>-0.01580481332099382</v>
@@ -6459,7 +6459,7 @@
         </is>
       </c>
       <c r="B96" s="1" t="n">
-        <v>-0.005417482741192137</v>
+        <v>-0.00541757091780215</v>
       </c>
       <c r="C96" s="1" t="n">
         <v>0.005464490366730912</v>
@@ -6484,7 +6484,7 @@
         </is>
       </c>
       <c r="B97" s="1" t="n">
-        <v>-0.002897396386007611</v>
+        <v>-0.002897307985966657</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>-0.0006038785751414366</v>
@@ -6559,7 +6559,7 @@
         </is>
       </c>
       <c r="B100" s="1" t="n">
-        <v>0.01366609138782771</v>
+        <v>0.01366600279252395</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>0</v>
@@ -6584,7 +6584,7 @@
         </is>
       </c>
       <c r="B101" s="1" t="n">
-        <v>0.0006284122940518611</v>
+        <v>0.0006284997498586797</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>0.02293988219229592</v>
@@ -6709,7 +6709,7 @@
         </is>
       </c>
       <c r="B106" s="1" t="n">
-        <v>0.01410476516615367</v>
+        <v>0.01410485360781855</v>
       </c>
       <c r="C106" s="1" t="n">
         <v>0.01567210527368679</v>
@@ -6759,7 +6759,7 @@
         </is>
       </c>
       <c r="B108" s="1" t="n">
-        <v>0.01065960811133837</v>
+        <v>0.0106595199701387</v>
       </c>
       <c r="C108" s="1" t="n">
         <v>-0.0002967992879533421</v>
@@ -6784,7 +6784,7 @@
         </is>
       </c>
       <c r="B109" s="1" t="n">
-        <v>-0.0002820876661849825</v>
+        <v>-0.0002820013744546657</v>
       </c>
       <c r="C109" s="1" t="n">
         <v>-0.0127634408638676</v>
@@ -6809,7 +6809,7 @@
         </is>
       </c>
       <c r="B110" s="1" t="n">
-        <v>0.01602259478735468</v>
+        <v>0.01602250708827579</v>
       </c>
       <c r="C110" s="1" t="n">
         <v>0.007817262457952001</v>
@@ -6884,7 +6884,7 @@
         </is>
       </c>
       <c r="B113" s="1" t="n">
-        <v>-0.002060383621211082</v>
+        <v>-0.002060298425064055</v>
       </c>
       <c r="C113" s="1" t="n">
         <v>0.002063062015756678</v>
@@ -6909,7 +6909,7 @@
         </is>
       </c>
       <c r="B114" s="1" t="n">
-        <v>-0.007756221146382636</v>
+        <v>-0.007756305856257195</v>
       </c>
       <c r="C114" s="1" t="n">
         <v>0.002941131591796875</v>
@@ -6984,7 +6984,7 @@
         </is>
       </c>
       <c r="B117" s="1" t="n">
-        <v>0.01563872426522583</v>
+        <v>0.01563880881166679</v>
       </c>
       <c r="C117" s="1" t="n">
         <v>0.008985547051913567</v>
@@ -7009,7 +7009,7 @@
         </is>
       </c>
       <c r="B118" s="1" t="n">
-        <v>-0.002611549639047195</v>
+        <v>-0.002611715910839085</v>
       </c>
       <c r="C118" s="1" t="n">
         <v>0.01350179222820946</v>
@@ -7034,7 +7034,7 @@
         </is>
       </c>
       <c r="B119" s="1" t="n">
-        <v>0.003491322688906839</v>
+        <v>0.003491406442876821</v>
       </c>
       <c r="C119" s="1" t="n">
         <v>0.003684837659107876</v>
@@ -7059,7 +7059,7 @@
         </is>
       </c>
       <c r="B120" s="1" t="n">
-        <v>0.01119863597612958</v>
+        <v>0.01119871914831672</v>
       </c>
       <c r="C120" s="1" t="n">
         <v>0.00169447538970835</v>
@@ -7084,7 +7084,7 @@
         </is>
       </c>
       <c r="B121" s="1" t="n">
-        <v>-0.005859896459041392</v>
+        <v>-0.005859978228138996</v>
       </c>
       <c r="C121" s="1" t="n">
         <v>0.0005638696666296905</v>
@@ -7184,7 +7184,7 @@
         </is>
       </c>
       <c r="B125" s="1" t="n">
-        <v>0.01652533153957325</v>
+        <v>0.01652524837190983</v>
       </c>
       <c r="C125" s="1" t="n">
         <v>-0.005196313751367199</v>
@@ -7209,7 +7209,7 @@
         </is>
       </c>
       <c r="B126" s="1" t="n">
-        <v>-0.001711337593146123</v>
+        <v>-0.001711255917520638</v>
       </c>
       <c r="C126" s="1" t="n">
         <v>-0.004643060117903608</v>
@@ -7234,7 +7234,7 @@
         </is>
       </c>
       <c r="B127" s="1" t="n">
-        <v>-0.007552890641506438</v>
+        <v>-0.007552972597393515</v>
       </c>
       <c r="C127" s="1" t="n">
         <v>0.002332414951433881</v>
@@ -7259,7 +7259,7 @@
         </is>
       </c>
       <c r="B128" s="1" t="n">
-        <v>0.01505896844203991</v>
+        <v>0.01505905226521231</v>
       </c>
       <c r="C128" s="1" t="n">
         <v>0.01076203956921651</v>
@@ -7334,7 +7334,7 @@
         </is>
       </c>
       <c r="B131" s="1" t="n">
-        <v>0.02310261358075549</v>
+        <v>0.02310253288280206</v>
       </c>
       <c r="C131" s="1" t="n">
         <v>0.02059759383026138</v>
@@ -7359,7 +7359,7 @@
         </is>
       </c>
       <c r="B132" s="1" t="n">
-        <v>-0.00778471787693702</v>
+        <v>-0.007784639615237898</v>
       </c>
       <c r="C132" s="1" t="n">
         <v>-0.01620237890504961</v>
@@ -7509,7 +7509,7 @@
         </is>
       </c>
       <c r="B138" s="1" t="n">
-        <v>-0.002809982450284298</v>
+        <v>-0.002810063567528331</v>
       </c>
       <c r="C138" s="1" t="n">
         <v>0.002680969717189674</v>
@@ -7534,7 +7534,7 @@
         </is>
       </c>
       <c r="B139" s="1" t="n">
-        <v>0.008985459759278225</v>
+        <v>0.008985541836038946</v>
       </c>
       <c r="C139" s="1" t="n">
         <v>0.01633984668906141</v>
@@ -7559,7 +7559,7 @@
         </is>
       </c>
       <c r="B140" s="1" t="n">
-        <v>0.004057433398255039</v>
+        <v>0.004057514019659036</v>
       </c>
       <c r="C140" s="1" t="n">
         <v>-0.005846266246473886</v>
@@ -7584,7 +7584,7 @@
         </is>
       </c>
       <c r="B141" s="1" t="n">
-        <v>0.0007872984550081341</v>
+        <v>0.000787298391791369</v>
       </c>
       <c r="C141" s="1" t="n">
         <v>0.002646285122893</v>
@@ -7609,7 +7609,7 @@
         </is>
       </c>
       <c r="B142" s="1" t="n">
-        <v>0.01730565656374394</v>
+        <v>0.01730549471039589</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>-0.006158331198519718</v>
@@ -7634,7 +7634,7 @@
         </is>
       </c>
       <c r="B143" s="1" t="n">
-        <v>-0.001340354651768072</v>
+        <v>-0.001340275889884723</v>
       </c>
       <c r="C143" s="1" t="n">
         <v>0.004130994162578894</v>
@@ -7759,7 +7759,7 @@
         </is>
       </c>
       <c r="B148" s="1" t="n">
-        <v>0.004513657295896589</v>
+        <v>0.004513577920933098</v>
       </c>
       <c r="C148" s="1" t="n">
         <v>0.001424588431098606</v>
@@ -7784,7 +7784,7 @@
         </is>
       </c>
       <c r="B149" s="1" t="n">
-        <v>0.004544974688857506</v>
+        <v>0.004545054066301901</v>
       </c>
       <c r="C149" s="1" t="n">
         <v>-0.01308685289334188</v>
@@ -7909,7 +7909,7 @@
         </is>
       </c>
       <c r="B154" s="1" t="n">
-        <v>-0.01549005444897344</v>
+        <v>-0.01548997623454629</v>
       </c>
       <c r="C154" s="1" t="n">
         <v>-0.002868682933661937</v>
@@ -7934,7 +7934,7 @@
         </is>
       </c>
       <c r="B155" s="1" t="n">
-        <v>-0.007321574991465574</v>
+        <v>-0.007321653854831633</v>
       </c>
       <c r="C155" s="1" t="n">
         <v>-0.01467198924509927</v>
@@ -8034,7 +8034,7 @@
         </is>
       </c>
       <c r="B159" s="1" t="n">
-        <v>-0.008954391503947501</v>
+        <v>-0.008954306412041091</v>
       </c>
       <c r="C159" s="1" t="n">
         <v>0.007615762767392065</v>
@@ -8059,7 +8059,7 @@
         </is>
       </c>
       <c r="B160" s="1" t="n">
-        <v>-0.001234591539437502</v>
+        <v>-0.001234677294164377</v>
       </c>
       <c r="C160" s="1" t="n">
         <v>-0.02180232461431086</v>

</xml_diff>

<commit_message>
Added line plots to PortfolioAnalyser
</commit_message>
<xml_diff>
--- a/Output/portfolio_overview.xlsx
+++ b/Output/portfolio_overview.xlsx
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3030152118272</v>
+        <v>3062035382272</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2754544140288</v>
+        <v>2774908534784</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>257444970496</v>
+        <v>258592260096</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>172864176128</v>
+        <v>172596969472</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>68587528192</v>
+        <v>68734943232</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>84970340352</v>
+        <v>85229002752</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -742,16 +742,16 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.5272385921430525</v>
+        <v>0.5272385921430498</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.2785967589266247</v>
+        <v>0.2785967589266225</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2042755514123077</v>
+        <v>0.2042756408268671</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>1.1352308466707</v>
+        <v>1.135231258552464</v>
       </c>
     </row>
     <row r="3">
@@ -764,16 +764,16 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.5955829673719624</v>
+        <v>0.5955829673719586</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.3358143391450037</v>
+        <v>0.3358143391450006</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2583212893345646</v>
+        <v>0.2583212849902302</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>1.23181213335027</v>
+        <v>1.231811604320493</v>
       </c>
     </row>
     <row r="4">
@@ -890,7 +890,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.3" customWidth="1" min="1" max="1"/>
-    <col width="29.26" customWidth="1" min="2" max="2"/>
+    <col width="27.93" customWidth="1" min="2" max="2"/>
     <col width="27.93" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -944,7 +944,7 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.006612899695142005</v>
+        <v>0.006612910404221628</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0.007538970575044379</v>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>-0.002080982315909363</v>
+        <v>-0.002080982638230422</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>-0.004194353599094369</v>
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.01084165316257013</v>
+        <v>0.0108416502150257</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.01855062511822725</v>
@@ -983,7 +983,7 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0.01777193604714156</v>
+        <v>0.01777196781309653</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0.01776875250938836</v>
@@ -996,7 +996,7 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.01478154858869174</v>
+        <v>0.01478154858882941</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.02487098016640643</v>
@@ -1009,7 +1009,7 @@
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.03341210176502574</v>
+        <v>0.03341210176516607</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.03803998256603447</v>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0.04018877994071191</v>
+        <v>0.04018879118658392</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0.04158582943200351</v>
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.04343310506106768</v>
+        <v>0.04343309636878145</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0.04574890046570768</v>
@@ -1048,7 +1048,7 @@
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>0.05273371660000614</v>
+        <v>0.05273370783024145</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0.04574890046570768</v>
@@ -1061,7 +1061,7 @@
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.05622000249238024</v>
+        <v>0.05621997123503886</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.04362551653740021</v>
@@ -1074,7 +1074,7 @@
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.04634424435805085</v>
+        <v>0.04634424421814698</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0.02738399163874461</v>
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.03448886093876169</v>
+        <v>0.03448884941591324</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.01953647282180282</v>
@@ -1100,7 +1100,7 @@
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.0483672513110871</v>
+        <v>0.04836725960021937</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.03882447269565104</v>
@@ -1113,7 +1113,7 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.06164291574246938</v>
+        <v>0.06164291554058154</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.05116710463322227</v>
@@ -1126,7 +1126,7 @@
         </is>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.06189512421395782</v>
+        <v>0.06189511278340731</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0.05041919595252109</v>
@@ -1139,7 +1139,7 @@
         </is>
       </c>
       <c r="B19" s="1" t="n">
-        <v>0.05897100336214178</v>
+        <v>0.05897098409983537</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0.05022830846167192</v>
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>0.06184317556723529</v>
+        <v>0.06184316433356951</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.06178906779040427</v>
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>0.06403372291202536</v>
+        <v>0.06403370378467721</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0.06443806265923357</v>
@@ -1178,7 +1178,7 @@
         </is>
       </c>
       <c r="B22" s="1" t="n">
-        <v>0.06186363741104906</v>
+        <v>0.06186362894917452</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0.05063364113036783</v>
@@ -1191,7 +1191,7 @@
         </is>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.0609430964079174</v>
+        <v>0.06094308442883323</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>0.06601751300157654</v>
@@ -1204,7 +1204,7 @@
         </is>
       </c>
       <c r="B24" s="1" t="n">
-        <v>0.06287619113371679</v>
+        <v>0.06287616054798417</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>0.07715985205772524</v>
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="B25" s="1" t="n">
-        <v>0.06896956731014159</v>
+        <v>0.06896956722733849</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>0.09299342676690747</v>
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="B26" s="1" t="n">
-        <v>0.08239078526803434</v>
+        <v>0.08239082404036258</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>0.08167590534457481</v>
@@ -1243,7 +1243,7 @@
         </is>
       </c>
       <c r="B27" s="1" t="n">
-        <v>0.07149575598876123</v>
+        <v>0.07149576257574952</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>0.07503391445061047</v>
@@ -1256,7 +1256,7 @@
         </is>
       </c>
       <c r="B28" s="1" t="n">
-        <v>0.07876172017029659</v>
+        <v>0.07876171284432765</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>0.08887229990761392</v>
@@ -1269,7 +1269,7 @@
         </is>
       </c>
       <c r="B29" s="1" t="n">
-        <v>0.07586911303066191</v>
+        <v>0.07586910907589139</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>0.07680680596260991</v>
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B30" s="1" t="n">
-        <v>0.07434484314947065</v>
+        <v>0.07434487789240896</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>0.06729882134316201</v>
@@ -1295,7 +1295,7 @@
         </is>
       </c>
       <c r="B31" s="1" t="n">
-        <v>0.07177651565774168</v>
+        <v>0.07177653201730649</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>0.0696418216489012</v>
@@ -1308,7 +1308,7 @@
         </is>
       </c>
       <c r="B32" s="1" t="n">
-        <v>0.08713295192763204</v>
+        <v>0.08713295005795474</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0.08188773300164431</v>
@@ -1321,7 +1321,7 @@
         </is>
       </c>
       <c r="B33" s="1" t="n">
-        <v>0.08873636065892376</v>
+        <v>0.08873635878648889</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>0.08158435595933167</v>
@@ -1334,7 +1334,7 @@
         </is>
       </c>
       <c r="B34" s="1" t="n">
-        <v>0.09373299852812367</v>
+        <v>0.09373301717360638</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>0.08458377940249884</v>
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="B35" s="1" t="n">
-        <v>0.0789182597203324</v>
+        <v>0.07891827585951816</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>0.06962873404501346</v>
@@ -1360,7 +1360,7 @@
         </is>
       </c>
       <c r="B36" s="1" t="n">
-        <v>0.078333766722259</v>
+        <v>0.07833378613099096</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>0.06666863725547945</v>
@@ -1373,7 +1373,7 @@
         </is>
       </c>
       <c r="B37" s="1" t="n">
-        <v>0.07655241037835037</v>
+        <v>0.07655242975501997</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>0.06666863725547945</v>
@@ -1386,7 +1386,7 @@
         </is>
       </c>
       <c r="B38" s="1" t="n">
-        <v>0.06870891526869505</v>
+        <v>0.06870891359709419</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>0.04529128122343162</v>
@@ -1399,7 +1399,7 @@
         </is>
       </c>
       <c r="B39" s="1" t="n">
-        <v>0.06822469357142413</v>
+        <v>0.06822469945458121</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>0.04364645670362055</v>
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B40" s="1" t="n">
-        <v>0.06988452103764953</v>
+        <v>0.06988452701056502</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>0.04920849682995865</v>
@@ -1425,7 +1425,7 @@
         </is>
       </c>
       <c r="B41" s="1" t="n">
-        <v>0.06001692998267272</v>
+        <v>0.0600169392047174</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>0.03815240827552802</v>
@@ -1438,7 +1438,7 @@
         </is>
       </c>
       <c r="B42" s="1" t="n">
-        <v>0.06571899623721333</v>
+        <v>0.06571899458236308</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>0.0413426553675742</v>
@@ -1451,7 +1451,7 @@
         </is>
       </c>
       <c r="B43" s="1" t="n">
-        <v>0.05870477703652832</v>
+        <v>0.0587047644896932</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>0.03818113716211058</v>
@@ -1464,7 +1464,7 @@
         </is>
       </c>
       <c r="B44" s="1" t="n">
-        <v>0.05151451930282991</v>
+        <v>0.05151448836504535</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>0.0332754563312303</v>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="B45" s="1" t="n">
-        <v>0.06089638722913282</v>
+        <v>0.06089636723385028</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>0.04110995138625473</v>
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="B46" s="1" t="n">
-        <v>0.07442552423564397</v>
+        <v>0.07442550463684716</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>0.05792152123667993</v>
@@ -1503,7 +1503,7 @@
         </is>
       </c>
       <c r="B47" s="1" t="n">
-        <v>0.07583401536980849</v>
+        <v>0.07583399608209129</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>0.05864848975116099</v>
@@ -1516,7 +1516,7 @@
         </is>
       </c>
       <c r="B48" s="1" t="n">
-        <v>0.06756328497268815</v>
+        <v>0.0675632941511537</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>0.04242266997717059</v>
@@ -1529,7 +1529,7 @@
         </is>
       </c>
       <c r="B49" s="1" t="n">
-        <v>0.06677415632463379</v>
+        <v>0.06677415476506776</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>0.04389748333038268</v>
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="B50" s="1" t="n">
-        <v>0.06536570054999591</v>
+        <v>0.0653656989924889</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>0.02462780610197712</v>
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B51" s="1" t="n">
-        <v>0.04296911867716791</v>
+        <v>0.04296911715240359</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>0.009793102858287828</v>
@@ -1568,7 +1568,7 @@
         </is>
       </c>
       <c r="B52" s="1" t="n">
-        <v>0.03289153561408487</v>
+        <v>0.03289150543274588</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>0.00826855661030268</v>
@@ -1581,7 +1581,7 @@
         </is>
       </c>
       <c r="B53" s="1" t="n">
-        <v>0.05141982701719883</v>
+        <v>0.05141984558273616</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>0.02488145024951671</v>
@@ -1594,7 +1594,7 @@
         </is>
       </c>
       <c r="B54" s="1" t="n">
-        <v>0.03274315594910249</v>
+        <v>0.03274317381690173</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>0.01772687217694791</v>
@@ -1607,7 +1607,7 @@
         </is>
       </c>
       <c r="B55" s="1" t="n">
-        <v>0.06085881301907681</v>
+        <v>0.06085881065141496</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>0.03560019783349699</v>
@@ -1620,7 +1620,7 @@
         </is>
       </c>
       <c r="B56" s="1" t="n">
-        <v>0.05508450637031137</v>
+        <v>0.05508450401553699</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>0.02418844566317313</v>
@@ -1633,7 +1633,7 @@
         </is>
       </c>
       <c r="B57" s="1" t="n">
-        <v>0.05860877594394776</v>
+        <v>0.05860877163579348</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>0.0333225717052259</v>
@@ -1646,7 +1646,7 @@
         </is>
       </c>
       <c r="B58" s="1" t="n">
-        <v>0.0849917326334364</v>
+        <v>0.08499171095266234</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>0.04673736569006093</v>
@@ -1659,7 +1659,7 @@
         </is>
       </c>
       <c r="B59" s="1" t="n">
-        <v>0.07845149989353706</v>
+        <v>0.0784514956267639</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>0.02950469420430446</v>
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="B60" s="1" t="n">
-        <v>0.07361690844725466</v>
+        <v>0.07361690730299797</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>0.03257728054530196</v>
@@ -1685,7 +1685,7 @@
         </is>
       </c>
       <c r="B61" s="1" t="n">
-        <v>0.06630820139749205</v>
+        <v>0.06630820026102491</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>0.03840081738151224</v>
@@ -1698,7 +1698,7 @@
         </is>
       </c>
       <c r="B62" s="1" t="n">
-        <v>0.0798670202290046</v>
+        <v>0.07986705552185547</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>0.0401110160787912</v>
@@ -1711,7 +1711,7 @@
         </is>
       </c>
       <c r="B63" s="1" t="n">
-        <v>0.08725478138434317</v>
+        <v>0.08725477707304541</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>0.03847404412131272</v>
@@ -1724,7 +1724,7 @@
         </is>
       </c>
       <c r="B64" s="1" t="n">
-        <v>0.1049083926348011</v>
+        <v>0.1049084261231128</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>0.05325907831219889</v>
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="B65" s="1" t="n">
-        <v>0.118543894573496</v>
+        <v>0.1185439105791399</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>0.05927873768081326</v>
@@ -1750,7 +1750,7 @@
         </is>
       </c>
       <c r="B66" s="1" t="n">
-        <v>0.1323023089983602</v>
+        <v>0.1323023249256736</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>0.07457106016677861</v>
@@ -1763,7 +1763,7 @@
         </is>
       </c>
       <c r="B67" s="1" t="n">
-        <v>0.1301663659976422</v>
+        <v>0.1301664018630211</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>0.07854573354647099</v>
@@ -1776,7 +1776,7 @@
         </is>
       </c>
       <c r="B68" s="1" t="n">
-        <v>0.1270056270879321</v>
+        <v>0.1270056254063012</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>0.07229343403850752</v>
@@ -1789,7 +1789,7 @@
         </is>
       </c>
       <c r="B69" s="1" t="n">
-        <v>0.1207901234601261</v>
+        <v>0.1207901017006265</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>0.06962088148268042</v>
@@ -1802,7 +1802,7 @@
         </is>
       </c>
       <c r="B70" s="1" t="n">
-        <v>0.1308468193266965</v>
+        <v>0.1308468207628162</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>0.07344922906671192</v>
@@ -1815,7 +1815,7 @@
         </is>
       </c>
       <c r="B71" s="1" t="n">
-        <v>0.1308468193266965</v>
+        <v>0.1308468207628162</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>0.07344922906671192</v>
@@ -1828,7 +1828,7 @@
         </is>
       </c>
       <c r="B72" s="1" t="n">
-        <v>0.1264080057718706</v>
+        <v>0.1264080047590892</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>0.0745187097512281</v>
@@ -1841,7 +1841,7 @@
         </is>
       </c>
       <c r="B73" s="1" t="n">
-        <v>0.1266629789610043</v>
+        <v>0.1266629779479935</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>0.07447427573998033</v>
@@ -1854,7 +1854,7 @@
         </is>
       </c>
       <c r="B74" s="1" t="n">
-        <v>0.1340977151267637</v>
+        <v>0.1340977166059434</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>0.07003144919293147</v>
@@ -1867,7 +1867,7 @@
         </is>
       </c>
       <c r="B75" s="1" t="n">
-        <v>0.1426214450338019</v>
+        <v>0.1426214442934521</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>0.08422294458702062</v>
@@ -1880,7 +1880,7 @@
         </is>
       </c>
       <c r="B76" s="1" t="n">
-        <v>0.1509842087076343</v>
+        <v>0.150984207961866</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>0.08197928238688723</v>
@@ -1893,7 +1893,7 @@
         </is>
       </c>
       <c r="B77" s="1" t="n">
-        <v>0.1490113679595635</v>
+        <v>0.1490113672150732</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>0.08555647566021629</v>
@@ -1906,7 +1906,7 @@
         </is>
       </c>
       <c r="B78" s="1" t="n">
-        <v>0.1517258664094092</v>
+        <v>0.1517258656631602</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>0.08648486559062674</v>
@@ -1919,7 +1919,7 @@
         </is>
       </c>
       <c r="B79" s="1" t="n">
-        <v>0.1509651360866064</v>
+        <v>0.1509651734499584</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>0.08639331620538337</v>
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="B80" s="1" t="n">
-        <v>0.1453260269927801</v>
+        <v>0.1453259914206768</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>0.07992650767760279</v>
@@ -1945,7 +1945,7 @@
         </is>
       </c>
       <c r="B81" s="1" t="n">
-        <v>0.1454623698876254</v>
+        <v>0.1454623485758504</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>0.0809018852980683</v>
@@ -1958,7 +1958,7 @@
         </is>
       </c>
       <c r="B82" s="1" t="n">
-        <v>0.1487350816106745</v>
+        <v>0.1487350776759095</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>0.08182235882417599</v>
@@ -1971,7 +1971,7 @@
         </is>
       </c>
       <c r="B83" s="1" t="n">
-        <v>0.1543254024451493</v>
+        <v>0.1543254013142217</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>0.06471781817257805</v>
@@ -1984,7 +1984,7 @@
         </is>
       </c>
       <c r="B84" s="1" t="n">
-        <v>0.1611153486395707</v>
+        <v>0.1611153475019909</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>0.06062803772064451</v>
@@ -1997,7 +1997,7 @@
         </is>
       </c>
       <c r="B85" s="1" t="n">
-        <v>0.1716849195169681</v>
+        <v>0.171684918369033</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>0.08138044470656491</v>
@@ -2010,7 +2010,7 @@
         </is>
       </c>
       <c r="B86" s="1" t="n">
-        <v>0.1762257919148882</v>
+        <v>0.1762257533230067</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>0.09030529677035548</v>
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="B87" s="1" t="n">
-        <v>0.1750371734685108</v>
+        <v>0.1750371543921807</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>0.08988432281896475</v>
@@ -2036,7 +2036,7 @@
         </is>
       </c>
       <c r="B88" s="1" t="n">
-        <v>0.1710239873479793</v>
+        <v>0.1710239879107192</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>0.07725663648452352</v>
@@ -2049,7 +2049,7 @@
         </is>
       </c>
       <c r="B89" s="1" t="n">
-        <v>0.1679387602453382</v>
+        <v>0.1679387392465057</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>0.06971766590947914</v>
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B90" s="1" t="n">
-        <v>0.1586826187881474</v>
+        <v>0.1586826372991077</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>0.0619956604059182</v>
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="B91" s="1" t="n">
-        <v>0.1830787331997659</v>
+        <v>0.1830787323482685</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>0.08161576620866162</v>
@@ -2088,7 +2088,7 @@
         </is>
       </c>
       <c r="B92" s="1" t="n">
-        <v>0.1846097089678169</v>
+        <v>0.1846096886217741</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>0.08210479570026807</v>
@@ -2101,7 +2101,7 @@
         </is>
       </c>
       <c r="B93" s="1" t="n">
-        <v>0.1827438717406313</v>
+        <v>0.1827438316764678</v>
       </c>
       <c r="C93" s="1" t="n">
         <v>0.07714938197461474</v>
@@ -2114,7 +2114,7 @@
         </is>
       </c>
       <c r="B94" s="1" t="n">
-        <v>0.180276923899098</v>
+        <v>0.1802769240398989</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>0.08197928238688701</v>
@@ -2127,7 +2127,7 @@
         </is>
       </c>
       <c r="B95" s="1" t="n">
-        <v>0.1821337872773239</v>
+        <v>0.1821338047828052</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>0.08014357037622699</v>
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="B96" s="1" t="n">
-        <v>0.182004507127044</v>
+        <v>0.1820045247247291</v>
       </c>
       <c r="C96" s="1" t="n">
         <v>0.07843337167894782</v>
@@ -2153,7 +2153,7 @@
         </is>
       </c>
       <c r="B97" s="1" t="n">
-        <v>0.1813364130681305</v>
+        <v>0.1813363936593526</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>0.08162355492902362</v>
@@ -2166,7 +2166,7 @@
         </is>
       </c>
       <c r="B98" s="1" t="n">
-        <v>0.1803117947263511</v>
+        <v>0.1803117950179556</v>
       </c>
       <c r="C98" s="1" t="n">
         <v>0.07472530236674202</v>
@@ -2179,7 +2179,7 @@
         </is>
       </c>
       <c r="B99" s="1" t="n">
-        <v>0.1810470815948031</v>
+        <v>0.1810470818865895</v>
       </c>
       <c r="C99" s="1" t="n">
         <v>0.08750467722233957</v>
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="B100" s="1" t="n">
-        <v>0.186570603089746</v>
+        <v>0.186570620822101</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>0.09777621180518348</v>
@@ -2205,7 +2205,7 @@
         </is>
       </c>
       <c r="B101" s="1" t="n">
-        <v>0.1982221065032046</v>
+        <v>0.1982221071142669</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>0.09618897274247806</v>
@@ -2218,7 +2218,7 @@
         </is>
       </c>
       <c r="B102" s="1" t="n">
-        <v>0.1988314767832984</v>
+        <v>0.1988314773946716</v>
       </c>
       <c r="C102" s="1" t="n">
         <v>0.09635892006710689</v>
@@ -2231,7 +2231,7 @@
         </is>
       </c>
       <c r="B103" s="1" t="n">
-        <v>0.1880644868759753</v>
+        <v>0.1880644874818576</v>
       </c>
       <c r="C103" s="1" t="n">
         <v>0.08405555094119865</v>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="B104" s="1" t="n">
-        <v>0.1809656291385797</v>
+        <v>0.1809656297408417</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>0.0761217816225388</v>
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="B105" s="1" t="n">
-        <v>0.1841688763275178</v>
+        <v>0.1841688769314134</v>
       </c>
       <c r="C105" s="1" t="n">
         <v>0.08554600557710579</v>
@@ -2270,7 +2270,7 @@
         </is>
       </c>
       <c r="B106" s="1" t="n">
-        <v>0.1991529237937519</v>
+        <v>0.1991529069503113</v>
       </c>
       <c r="C106" s="1" t="n">
         <v>0.09971138960538983</v>
@@ -2283,7 +2283,7 @@
         </is>
       </c>
       <c r="B107" s="1" t="n">
-        <v>0.1991529237937519</v>
+        <v>0.1991529069503113</v>
       </c>
       <c r="C107" s="1" t="n">
         <v>0.09971138960538983</v>
@@ -2296,7 +2296,7 @@
         </is>
       </c>
       <c r="B108" s="1" t="n">
-        <v>0.1855950056166202</v>
+        <v>0.1855950065794116</v>
       </c>
       <c r="C108" s="1" t="n">
         <v>0.09972964840886234</v>
@@ -2309,7 +2309,7 @@
         </is>
       </c>
       <c r="B109" s="1" t="n">
-        <v>0.1770286294461185</v>
+        <v>0.1770286133507792</v>
       </c>
       <c r="C109" s="1" t="n">
         <v>0.09301181325431984</v>
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="B110" s="1" t="n">
-        <v>0.1925560778168005</v>
+        <v>0.1925560787131844</v>
       </c>
       <c r="C110" s="1" t="n">
         <v>0.1037828474118807</v>
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="B111" s="1" t="n">
-        <v>0.2069206344346712</v>
+        <v>0.2069206353418522</v>
       </c>
       <c r="C111" s="1" t="n">
         <v>0.1198256960993249</v>
@@ -2348,7 +2348,7 @@
         </is>
       </c>
       <c r="B112" s="1" t="n">
-        <v>0.2069869013047807</v>
+        <v>0.2069869022120114</v>
       </c>
       <c r="C112" s="1" t="n">
         <v>0.1175820338991915</v>
@@ -2361,7 +2361,7 @@
         </is>
       </c>
       <c r="B113" s="1" t="n">
-        <v>0.2081463950311888</v>
+        <v>0.208146378800852</v>
       </c>
       <c r="C113" s="1" t="n">
         <v>0.120212706122578</v>
@@ -2374,7 +2374,7 @@
         </is>
       </c>
       <c r="B114" s="1" t="n">
-        <v>0.1962757470622083</v>
+        <v>0.1962757480483308</v>
       </c>
       <c r="C114" s="1" t="n">
         <v>0.1159424444209354</v>
@@ -2387,7 +2387,7 @@
         </is>
       </c>
       <c r="B115" s="1" t="n">
-        <v>0.2015949272919013</v>
+        <v>0.2015949282824085</v>
       </c>
       <c r="C115" s="1" t="n">
         <v>0.1228486133875195</v>
@@ -2400,7 +2400,7 @@
         </is>
       </c>
       <c r="B116" s="1" t="n">
-        <v>0.2041863004351607</v>
+        <v>0.204186301427804</v>
       </c>
       <c r="C116" s="1" t="n">
         <v>0.1241377104494672</v>
@@ -2413,7 +2413,7 @@
         </is>
       </c>
       <c r="B117" s="1" t="n">
-        <v>0.2149338353356236</v>
+        <v>0.2149338193688484</v>
       </c>
       <c r="C117" s="1" t="n">
         <v>0.134615965331766</v>
@@ -2426,7 +2426,7 @@
         </is>
       </c>
       <c r="B118" s="1" t="n">
-        <v>0.2166332807891778</v>
+        <v>0.216633298468272</v>
       </c>
       <c r="C118" s="1" t="n">
         <v>0.1424816791102101</v>
@@ -2439,7 +2439,7 @@
         </is>
       </c>
       <c r="B119" s="1" t="n">
-        <v>0.2195718349262605</v>
+        <v>0.2195718356650771</v>
       </c>
       <c r="C119" s="1" t="n">
         <v>0.1434178577609828</v>
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="B120" s="1" t="n">
-        <v>0.2304278963600734</v>
+        <v>0.2304278801997239</v>
       </c>
       <c r="C120" s="1" t="n">
         <v>0.1573425575616745</v>
@@ -2465,7 +2465,7 @@
         </is>
       </c>
       <c r="B121" s="1" t="n">
-        <v>0.2270374625248637</v>
+        <v>0.2270374631775403</v>
       </c>
       <c r="C121" s="1" t="n">
         <v>0.1530932360262522</v>
@@ -2478,7 +2478,7 @@
         </is>
       </c>
       <c r="B122" s="1" t="n">
-        <v>0.2285436010888628</v>
+        <v>0.2285436017423406</v>
       </c>
       <c r="C122" s="1" t="n">
         <v>0.1530932360262522</v>
@@ -2491,7 +2491,7 @@
         </is>
       </c>
       <c r="B123" s="1" t="n">
-        <v>0.2166679197033814</v>
+        <v>0.2166679203505424</v>
       </c>
       <c r="C123" s="1" t="n">
         <v>0.1476332153682676</v>
@@ -2504,7 +2504,7 @@
         </is>
       </c>
       <c r="B124" s="1" t="n">
-        <v>0.2128756085927308</v>
+        <v>0.2128756092378745</v>
       </c>
       <c r="C124" s="1" t="n">
         <v>0.1416135559996532</v>
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="B125" s="1" t="n">
-        <v>0.2158842884634427</v>
+        <v>0.215884305922192</v>
       </c>
       <c r="C125" s="1" t="n">
         <v>0.1458498537731581</v>
@@ -2530,7 +2530,7 @@
         </is>
       </c>
       <c r="B126" s="1" t="n">
-        <v>0.2130905672232486</v>
+        <v>0.2130905680905313</v>
       </c>
       <c r="C126" s="1" t="n">
         <v>0.137074008867776</v>
@@ -2543,7 +2543,7 @@
         </is>
       </c>
       <c r="B127" s="1" t="n">
-        <v>0.2008828554801452</v>
+        <v>0.2008828729086858</v>
       </c>
       <c r="C127" s="1" t="n">
         <v>0.1319721416625215</v>
@@ -2556,7 +2556,7 @@
         </is>
       </c>
       <c r="B128" s="1" t="n">
-        <v>0.2091656246656379</v>
+        <v>0.2091656254374186</v>
       </c>
       <c r="C128" s="1" t="n">
         <v>0.1449398503301607</v>
@@ -2569,7 +2569,7 @@
         </is>
       </c>
       <c r="B129" s="1" t="n">
-        <v>0.2126337692459865</v>
+        <v>0.2126337700199807</v>
       </c>
       <c r="C129" s="1" t="n">
         <v>0.1445344538194946</v>
@@ -2582,7 +2582,7 @@
         </is>
       </c>
       <c r="B130" s="1" t="n">
-        <v>0.2122480502441118</v>
+        <v>0.2122480510178597</v>
       </c>
       <c r="C130" s="1" t="n">
         <v>0.1496545798282216</v>
@@ -2595,7 +2595,7 @@
         </is>
       </c>
       <c r="B131" s="1" t="n">
-        <v>0.2299601237546056</v>
+        <v>0.2299601408439815</v>
       </c>
       <c r="C131" s="1" t="n">
         <v>0.1637596970366524</v>
@@ -2608,7 +2608,7 @@
         </is>
       </c>
       <c r="B132" s="1" t="n">
-        <v>0.2227355499091326</v>
+        <v>0.222735550855</v>
       </c>
       <c r="C132" s="1" t="n">
         <v>0.1651220846803712</v>
@@ -2621,7 +2621,7 @@
         </is>
       </c>
       <c r="B133" s="1" t="n">
-        <v>0.21981163369005</v>
+        <v>0.2198116346336554</v>
       </c>
       <c r="C133" s="1" t="n">
         <v>0.1651220846803712</v>
@@ -2634,7 +2634,7 @@
         </is>
       </c>
       <c r="B134" s="1" t="n">
-        <v>0.2151920758824546</v>
+        <v>0.2151920768224864</v>
       </c>
       <c r="C134" s="1" t="n">
         <v>0.1628287534274349</v>
@@ -2647,7 +2647,7 @@
         </is>
       </c>
       <c r="B135" s="1" t="n">
-        <v>0.2023788598816356</v>
+        <v>0.2023788608117554</v>
       </c>
       <c r="C135" s="1" t="n">
         <v>0.1536162294459968</v>
@@ -2660,7 +2660,7 @@
         </is>
       </c>
       <c r="B136" s="1" t="n">
-        <v>0.1932247608632767</v>
+        <v>0.1932247617863152</v>
       </c>
       <c r="C136" s="1" t="n">
         <v>0.15031100296565</v>
@@ -2673,7 +2673,7 @@
         </is>
       </c>
       <c r="B137" s="1" t="n">
-        <v>0.1921795585147321</v>
+        <v>0.1921795594369622</v>
       </c>
       <c r="C137" s="1" t="n">
         <v>0.1530775309015873</v>
@@ -2686,7 +2686,7 @@
         </is>
       </c>
       <c r="B138" s="1" t="n">
-        <v>0.192287806167921</v>
+        <v>0.1922878232079546</v>
       </c>
       <c r="C138" s="1" t="n">
         <v>0.1608518229787286</v>
@@ -2699,7 +2699,7 @@
         </is>
       </c>
       <c r="B139" s="1" t="n">
-        <v>0.2008750524257745</v>
+        <v>0.2008750532786825</v>
       </c>
       <c r="C139" s="1" t="n">
         <v>0.1694551668806745</v>
@@ -2712,7 +2712,7 @@
         </is>
       </c>
       <c r="B140" s="1" t="n">
-        <v>0.2039303270941917</v>
+        <v>0.2039303118132307</v>
       </c>
       <c r="C140" s="1" t="n">
         <v>0.1793606316064857</v>
@@ -2725,7 +2725,7 @@
         </is>
       </c>
       <c r="B141" s="1" t="n">
-        <v>0.2070084864458552</v>
+        <v>0.2070084711385092</v>
       </c>
       <c r="C141" s="1" t="n">
         <v>0.1781524861627306</v>
@@ -2738,7 +2738,7 @@
         </is>
       </c>
       <c r="B142" s="1" t="n">
-        <v>0.2091184569253735</v>
+        <v>0.2091184741509955</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>0.1826947146573554</v>
@@ -2751,7 +2751,7 @@
         </is>
       </c>
       <c r="B143" s="1" t="n">
-        <v>0.2284148294230193</v>
+        <v>0.2284148310514713</v>
       </c>
       <c r="C143" s="1" t="n">
         <v>0.191112278426067</v>
@@ -2764,7 +2764,7 @@
         </is>
       </c>
       <c r="B144" s="1" t="n">
-        <v>0.2252055896220522</v>
+        <v>0.2252055912462498</v>
       </c>
       <c r="C144" s="1" t="n">
         <v>0.1939208143783853</v>
@@ -2777,7 +2777,7 @@
         </is>
       </c>
       <c r="B145" s="1" t="n">
-        <v>0.228881276346254</v>
+        <v>0.2288812779753244</v>
       </c>
       <c r="C145" s="1" t="n">
         <v>0.1858536153420414</v>
@@ -2790,7 +2790,7 @@
         </is>
       </c>
       <c r="B146" s="1" t="n">
-        <v>0.2307000724928527</v>
+        <v>0.2307000741243344</v>
       </c>
       <c r="C146" s="1" t="n">
         <v>0.1862379440025468</v>
@@ -2803,7 +2803,7 @@
         </is>
       </c>
       <c r="B147" s="1" t="n">
-        <v>0.2336397189127075</v>
+        <v>0.233639720548086</v>
       </c>
       <c r="C147" s="1" t="n">
         <v>0.1910234104035713</v>
@@ -2816,7 +2816,7 @@
         </is>
       </c>
       <c r="B148" s="1" t="n">
-        <v>0.240339248238302</v>
+        <v>0.2403392662025798</v>
       </c>
       <c r="C148" s="1" t="n">
         <v>0.1943757522579137</v>
@@ -2829,7 +2829,7 @@
         </is>
       </c>
       <c r="B149" s="1" t="n">
-        <v>0.2306476165561282</v>
+        <v>0.2306476179708783</v>
       </c>
       <c r="C149" s="1" t="n">
         <v>0.1941900998086197</v>
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="B150" s="1" t="n">
-        <v>0.2389747405825895</v>
+        <v>0.2389747420069126</v>
       </c>
       <c r="C150" s="1" t="n">
         <v>0.1865178271998318</v>
@@ -2855,7 +2855,7 @@
         </is>
       </c>
       <c r="B151" s="1" t="n">
-        <v>0.2433521189250101</v>
+        <v>0.2433521203543654</v>
       </c>
       <c r="C151" s="1" t="n">
         <v>0.1982380637700829</v>
@@ -2868,7 +2868,7 @@
         </is>
       </c>
       <c r="B152" s="1" t="n">
-        <v>0.243495690575511</v>
+        <v>0.2434956920050313</v>
       </c>
       <c r="C152" s="1" t="n">
         <v>0.1999979315201648</v>
@@ -2881,7 +2881,7 @@
         </is>
       </c>
       <c r="B153" s="1" t="n">
-        <v>0.2428686193410912</v>
+        <v>0.2428686207698907</v>
       </c>
       <c r="C153" s="1" t="n">
         <v>0.196799831865786</v>
@@ -2894,7 +2894,7 @@
         </is>
       </c>
       <c r="B154" s="1" t="n">
-        <v>0.2286255203033287</v>
+        <v>0.2286255055140449</v>
       </c>
       <c r="C154" s="1" t="n">
         <v>0.1802366711213452</v>
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="B155" s="1" t="n">
-        <v>0.2175837628328792</v>
+        <v>0.2175837643254319</v>
       </c>
       <c r="C155" s="1" t="n">
         <v>0.1772294589578156</v>
@@ -2920,7 +2920,7 @@
         </is>
       </c>
       <c r="B156" s="1" t="n">
-        <v>0.2108996473486549</v>
+        <v>0.2108996488330139</v>
       </c>
       <c r="C156" s="1" t="n">
         <v>0.1709900555278292</v>
@@ -2933,7 +2933,7 @@
         </is>
       </c>
       <c r="B157" s="1" t="n">
-        <v>0.2127630254748381</v>
+        <v>0.2127630269614813</v>
       </c>
       <c r="C157" s="1" t="n">
         <v>0.1815571784326235</v>
@@ -2946,7 +2946,7 @@
         </is>
       </c>
       <c r="B158" s="1" t="n">
-        <v>0.2060625134772445</v>
+        <v>0.2060625149556741</v>
       </c>
       <c r="C158" s="1" t="n">
         <v>0.1765730358203876</v>
@@ -2959,7 +2959,7 @@
         </is>
       </c>
       <c r="B159" s="1" t="n">
-        <v>0.2074786490860936</v>
+        <v>0.2074786334618992</v>
       </c>
       <c r="C159" s="1" t="n">
         <v>0.1682914554481674</v>
@@ -2972,7 +2972,7 @@
         </is>
       </c>
       <c r="B160" s="1" t="n">
-        <v>0.205393167485902</v>
+        <v>0.2053931691465261</v>
       </c>
       <c r="C160" s="1" t="n">
         <v>0.16858436240737</v>
@@ -2985,7 +2985,7 @@
         </is>
       </c>
       <c r="B161" s="1" t="n">
-        <v>0.2133022115921965</v>
+        <v>0.2133022132637168</v>
       </c>
       <c r="C161" s="1" t="n">
         <v>0.1673343366311746</v>
@@ -2998,7 +2998,7 @@
         </is>
       </c>
       <c r="B162" s="1" t="n">
-        <v>0.2230964570561804</v>
+        <v>0.2230964587411937</v>
       </c>
       <c r="C162" s="1" t="n">
         <v>0.1740470644281025</v>
@@ -3011,7 +3011,7 @@
         </is>
       </c>
       <c r="B163" s="1" t="n">
-        <v>0.2111481758809077</v>
+        <v>0.2111481775494604</v>
       </c>
       <c r="C163" s="1" t="n">
         <v>0.1604857531216959</v>
@@ -3024,7 +3024,7 @@
         </is>
       </c>
       <c r="B164" s="1" t="n">
-        <v>0.2130502016389548</v>
+        <v>0.2130502033101278</v>
       </c>
       <c r="C164" s="1" t="n">
         <v>0.1517178246206166</v>
@@ -3037,7 +3037,7 @@
         </is>
       </c>
       <c r="B165" s="1" t="n">
-        <v>0.19998163334636</v>
+        <v>0.1999816349995287</v>
       </c>
       <c r="C165" s="1" t="n">
         <v>0.1428347252053261</v>
@@ -3050,7 +3050,7 @@
         </is>
       </c>
       <c r="B166" s="1" t="n">
-        <v>0.1994144942269851</v>
+        <v>0.1994144958793724</v>
       </c>
       <c r="C166" s="1" t="n">
         <v>0.1426647778806973</v>
@@ -3063,7 +3063,7 @@
         </is>
       </c>
       <c r="B167" s="1" t="n">
-        <v>0.2050930058359608</v>
+        <v>0.2050930074961712</v>
       </c>
       <c r="C167" s="1" t="n">
         <v>0.1505253843015268</v>
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="B168" s="1" t="n">
-        <v>0.2145557931426245</v>
+        <v>0.2145557948158716</v>
       </c>
       <c r="C168" s="1" t="n">
         <v>0.1473298383259554</v>
@@ -3089,7 +3089,7 @@
         </is>
       </c>
       <c r="B169" s="1" t="n">
-        <v>0.2259554383630162</v>
+        <v>0.2259554400519681</v>
       </c>
       <c r="C169" s="1" t="n">
         <v>0.1600019586716444</v>
@@ -3102,7 +3102,7 @@
         </is>
       </c>
       <c r="B170" s="1" t="n">
-        <v>0.222453129168352</v>
+        <v>0.2224531308524789</v>
       </c>
       <c r="C170" s="1" t="n">
         <v>0.1443906817026415</v>
@@ -3115,7 +3115,7 @@
         </is>
       </c>
       <c r="B171" s="1" t="n">
-        <v>0.225382157204097</v>
+        <v>0.2253821588922591</v>
       </c>
       <c r="C171" s="1" t="n">
         <v>0.1520786594360943</v>
@@ -3128,7 +3128,7 @@
         </is>
       </c>
       <c r="B172" s="1" t="n">
-        <v>0.2359789199727427</v>
+        <v>0.2359789216755035</v>
       </c>
       <c r="C172" s="1" t="n">
         <v>0.1592959941653536</v>
@@ -3141,7 +3141,7 @@
         </is>
       </c>
       <c r="B173" s="1" t="n">
-        <v>0.2470658533829719</v>
+        <v>0.2470658551010068</v>
       </c>
       <c r="C173" s="1" t="n">
         <v>0.1761154165781114</v>
@@ -3154,7 +3154,7 @@
         </is>
       </c>
       <c r="B174" s="1" t="n">
-        <v>0.2494882240835337</v>
+        <v>0.2494882258049058</v>
       </c>
       <c r="C174" s="1" t="n">
         <v>0.1806236811445985</v>
@@ -3167,7 +3167,7 @@
         </is>
       </c>
       <c r="B175" s="1" t="n">
-        <v>0.2607031297877309</v>
+        <v>0.2607031315245534</v>
       </c>
       <c r="C175" s="1" t="n">
         <v>0.1787383000811356</v>
@@ -3180,7 +3180,7 @@
         </is>
       </c>
       <c r="B176" s="1" t="n">
-        <v>0.2582109507217925</v>
+        <v>0.2582109524551814</v>
       </c>
       <c r="C176" s="1" t="n">
         <v>0.1808590026466954</v>
@@ -3193,7 +3193,7 @@
         </is>
       </c>
       <c r="B177" s="1" t="n">
-        <v>0.259284346025586</v>
+        <v>0.2592843477604538</v>
       </c>
       <c r="C177" s="1" t="n">
         <v>0.1808590026466954</v>
@@ -3206,7 +3206,7 @@
         </is>
       </c>
       <c r="B178" s="1" t="n">
-        <v>0.2549084249362037</v>
+        <v>0.254908426665043</v>
       </c>
       <c r="C178" s="1" t="n">
         <v>0.1759062702837899</v>
@@ -3219,7 +3219,7 @@
         </is>
       </c>
       <c r="B179" s="1" t="n">
-        <v>0.2446898522236813</v>
+        <v>0.2446898539384428</v>
       </c>
       <c r="C179" s="1" t="n">
         <v>0.16770832289251</v>
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="B180" s="1" t="n">
-        <v>0.2395406503945494</v>
+        <v>0.239540652102217</v>
       </c>
       <c r="C180" s="1" t="n">
         <v>0.1639585009318043</v>
@@ -3245,7 +3245,7 @@
         </is>
       </c>
       <c r="B181" s="1" t="n">
-        <v>0.2373376851041502</v>
+        <v>0.2373376868087829</v>
       </c>
       <c r="C181" s="1" t="n">
         <v>0.1656190305762804</v>
@@ -3258,7 +3258,7 @@
         </is>
       </c>
       <c r="B182" s="1" t="n">
-        <v>0.2450398355135575</v>
+        <v>0.245039837228801</v>
       </c>
       <c r="C182" s="1" t="n">
         <v>0.1734560154681419</v>
@@ -3271,7 +3271,7 @@
         </is>
       </c>
       <c r="B183" s="1" t="n">
-        <v>0.239286750761484</v>
+        <v>0.2392867524688018</v>
       </c>
       <c r="C183" s="1" t="n">
         <v>0.1667721442417371</v>
@@ -3284,7 +3284,7 @@
         </is>
       </c>
       <c r="B184" s="1" t="n">
-        <v>0.236111461837625</v>
+        <v>0.2361114635405686</v>
       </c>
       <c r="C184" s="1" t="n">
         <v>0.1682208462291439</v>
@@ -3297,7 +3297,7 @@
         </is>
       </c>
       <c r="B185" s="1" t="n">
-        <v>0.2480752910393571</v>
+        <v>0.2480752927587828</v>
       </c>
       <c r="C185" s="1" t="n">
         <v>0.1780688531817898</v>
@@ -3310,7 +3310,7 @@
         </is>
       </c>
       <c r="B186" s="1" t="n">
-        <v>0.2464589232968679</v>
+        <v>0.246458925014067</v>
       </c>
       <c r="C186" s="1" t="n">
         <v>0.1637439919119872</v>
@@ -3323,7 +3323,7 @@
         </is>
       </c>
       <c r="B187" s="1" t="n">
-        <v>0.2509667340331485</v>
+        <v>0.2509667357565577</v>
       </c>
       <c r="C187" s="1" t="n">
         <v>0.1645833861359616</v>
@@ -3336,7 +3336,7 @@
         </is>
       </c>
       <c r="B188" s="1" t="n">
-        <v>0.2491627870741235</v>
+        <v>0.2491627887950474</v>
       </c>
       <c r="C188" s="1" t="n">
         <v>0.1620783549098963</v>
@@ -3349,7 +3349,7 @@
         </is>
       </c>
       <c r="B189" s="1" t="n">
-        <v>0.2487867822240515</v>
+        <v>0.2487867839444575</v>
       </c>
       <c r="C189" s="1" t="n">
         <v>0.1511608672727343</v>
@@ -3362,7 +3362,7 @@
         </is>
       </c>
       <c r="B190" s="1" t="n">
-        <v>0.2424780280554886</v>
+        <v>0.2424780297672033</v>
       </c>
       <c r="C190" s="1" t="n">
         <v>0.1322807537463893</v>
@@ -3375,7 +3375,7 @@
         </is>
       </c>
       <c r="B191" s="1" t="n">
-        <v>0.234216955960947</v>
+        <v>0.2342169576612809</v>
       </c>
       <c r="C191" s="1" t="n">
         <v>0.129681491772333</v>
@@ -3388,7 +3388,7 @@
         </is>
       </c>
       <c r="B192" s="1" t="n">
-        <v>0.2390437741617208</v>
+        <v>0.2390437758687043</v>
       </c>
       <c r="C192" s="1" t="n">
         <v>0.1342262739457651</v>
@@ -3401,7 +3401,7 @@
         </is>
       </c>
       <c r="B193" s="1" t="n">
-        <v>0.2254389859787169</v>
+        <v>0.2254389876669576</v>
       </c>
       <c r="C193" s="1" t="n">
         <v>0.1175139783589754</v>
@@ -3414,7 +3414,7 @@
         </is>
       </c>
       <c r="B194" s="1" t="n">
-        <v>0.2163200372687477</v>
+        <v>0.2163200389444255</v>
       </c>
       <c r="C194" s="1" t="n">
         <v>0.1177702400272924</v>
@@ -3427,7 +3427,7 @@
         </is>
       </c>
       <c r="B195" s="1" t="n">
-        <v>0.2236003929609023</v>
+        <v>0.2236003946466099</v>
       </c>
       <c r="C195" s="1" t="n">
         <v>0.1243574545108392</v>
@@ -3440,7 +3440,7 @@
         </is>
       </c>
       <c r="B196" s="1" t="n">
-        <v>0.2272233373588368</v>
+        <v>0.2272233390495357</v>
       </c>
       <c r="C196" s="1" t="n">
         <v>0.1213109156936765</v>
@@ -3453,7 +3453,7 @@
         </is>
       </c>
       <c r="B197" s="1" t="n">
-        <v>0.2296566646658436</v>
+        <v>0.2296566663598947</v>
       </c>
       <c r="C197" s="1" t="n">
         <v>0.1213999114001123</v>
@@ -3466,7 +3466,7 @@
         </is>
       </c>
       <c r="B198" s="1" t="n">
-        <v>0.2134421744127453</v>
+        <v>0.2134421760844583</v>
       </c>
       <c r="C198" s="1" t="n">
         <v>0.1059873106423208</v>
@@ -3479,7 +3479,7 @@
         </is>
       </c>
       <c r="B199" s="1" t="n">
-        <v>0.219268645868165</v>
+        <v>0.2192686475479049</v>
       </c>
       <c r="C199" s="1" t="n">
         <v>0.1149565967173591</v>
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="B200" s="1" t="n">
-        <v>0.2203726925155822</v>
+        <v>0.2203726941968431</v>
       </c>
       <c r="C200" s="1" t="n">
         <v>0.1135026596883972</v>
@@ -3505,7 +3505,7 @@
         </is>
       </c>
       <c r="B201" s="1" t="n">
-        <v>0.232743052349792</v>
+        <v>0.232743054048095</v>
       </c>
       <c r="C201" s="1" t="n">
         <v>0.1266585744841378</v>
@@ -3518,7 +3518,7 @@
         </is>
       </c>
       <c r="B202" s="1" t="n">
-        <v>0.2319487190057634</v>
+        <v>0.2319487207029722</v>
       </c>
       <c r="C202" s="1" t="n">
         <v>0.1337608659831262</v>
@@ -3531,7 +3531,7 @@
         </is>
       </c>
       <c r="B203" s="1" t="n">
-        <v>0.2440446140221404</v>
+        <v>0.2440446157360134</v>
       </c>
       <c r="C203" s="1" t="n">
         <v>0.1396654821214696</v>
@@ -3544,7 +3544,7 @@
         </is>
       </c>
       <c r="B204" s="1" t="n">
-        <v>0.2565743383424974</v>
+        <v>0.2565743400736322</v>
       </c>
       <c r="C204" s="1" t="n">
         <v>0.1445580753484621</v>
@@ -3557,7 +3557,7 @@
         </is>
       </c>
       <c r="B205" s="1" t="n">
-        <v>0.2512946904036528</v>
+        <v>0.2512946921275141</v>
       </c>
       <c r="C205" s="1" t="n">
         <v>0.1374086684754783</v>
@@ -3570,7 +3570,7 @@
         </is>
       </c>
       <c r="B206" s="1" t="n">
-        <v>0.2345550243771251</v>
+        <v>0.2345550260779248</v>
       </c>
       <c r="C206" s="1" t="n">
         <v>0.131700174869539</v>
@@ -3583,7 +3583,7 @@
         </is>
       </c>
       <c r="B207" s="1" t="n">
-        <v>0.2385784480037272</v>
+        <v>0.2385784497100698</v>
       </c>
       <c r="C207" s="1" t="n">
         <v>0.1436898245539648</v>
@@ -3596,7 +3596,7 @@
         </is>
       </c>
       <c r="B208" s="1" t="n">
-        <v>0.2375097917048852</v>
+        <v>0.2375097934097554</v>
       </c>
       <c r="C208" s="1" t="n">
         <v>0.1435774626864417</v>
@@ -3609,7 +3609,7 @@
         </is>
       </c>
       <c r="B209" s="1" t="n">
-        <v>0.2149252627725664</v>
+        <v>0.2149252644463229</v>
       </c>
       <c r="C209" s="1" t="n">
         <v>0.1282537299511459</v>
@@ -3622,7 +3622,7 @@
         </is>
       </c>
       <c r="B210" s="1" t="n">
-        <v>0.1979306170626691</v>
+        <v>0.1979306187130128</v>
       </c>
       <c r="C210" s="1" t="n">
         <v>0.1186829248330374</v>
@@ -3635,7 +3635,7 @@
         </is>
       </c>
       <c r="B211" s="1" t="n">
-        <v>0.1814962389850474</v>
+        <v>0.18149624061275</v>
       </c>
       <c r="C211" s="1" t="n">
         <v>0.1046039828323821</v>
@@ -3648,7 +3648,7 @@
         </is>
       </c>
       <c r="B212" s="1" t="n">
-        <v>0.184519786267993</v>
+        <v>0.184519787899861</v>
       </c>
       <c r="C212" s="1" t="n">
         <v>0.1027420956139469</v>
@@ -3661,7 +3661,7 @@
         </is>
       </c>
       <c r="B213" s="1" t="n">
-        <v>0.1856383268160877</v>
+        <v>0.1856383284494967</v>
       </c>
       <c r="C213" s="1" t="n">
         <v>0.1107543905559327</v>
@@ -3674,7 +3674,7 @@
         </is>
       </c>
       <c r="B214" s="1" t="n">
-        <v>0.1952159043286872</v>
+        <v>0.1952159059752907</v>
       </c>
       <c r="C214" s="1" t="n">
         <v>0.09482658509875952</v>
@@ -3687,7 +3687,7 @@
         </is>
       </c>
       <c r="B215" s="1" t="n">
-        <v>0.1813233975396487</v>
+        <v>0.181323399167113</v>
       </c>
       <c r="C215" s="1" t="n">
         <v>0.08187202787697823</v>
@@ -3700,7 +3700,7 @@
         </is>
       </c>
       <c r="B216" s="1" t="n">
-        <v>0.1775656361579423</v>
+        <v>0.1775656377802297</v>
       </c>
       <c r="C216" s="1" t="n">
         <v>0.07667873897042088</v>
@@ -3713,7 +3713,7 @@
         </is>
       </c>
       <c r="B217" s="1" t="n">
-        <v>0.1872316822627926</v>
+        <v>0.1872316838983967</v>
       </c>
       <c r="C217" s="1" t="n">
         <v>0.08960967466323422</v>
@@ -3726,7 +3726,7 @@
         </is>
       </c>
       <c r="B218" s="1" t="n">
-        <v>0.191776820943935</v>
+        <v>0.1917768225858008</v>
       </c>
       <c r="C218" s="1" t="n">
         <v>0.09666485078822706</v>
@@ -3739,7 +3739,7 @@
         </is>
       </c>
       <c r="B219" s="1" t="n">
-        <v>0.2096168040625883</v>
+        <v>0.2096168057290315</v>
       </c>
       <c r="C219" s="1" t="n">
         <v>0.1081864111472668</v>
@@ -3752,7 +3752,7 @@
         </is>
       </c>
       <c r="B220" s="1" t="n">
-        <v>0.221006967257114</v>
+        <v>0.2210069689392489</v>
       </c>
       <c r="C220" s="1" t="n">
         <v>0.1290852077708182</v>
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="B221" s="1" t="n">
-        <v>0.2193269419045567</v>
+        <v>0.2193269435843772</v>
       </c>
       <c r="C221" s="1" t="n">
         <v>0.1396915296453052</v>
@@ -3778,7 +3778,7 @@
         </is>
       </c>
       <c r="B222" s="1" t="n">
-        <v>0.2257622057749158</v>
+        <v>0.2257622074636019</v>
       </c>
       <c r="C222" s="1" t="n">
         <v>0.1416894002602316</v>
@@ -3791,7 +3791,7 @@
         </is>
       </c>
       <c r="B223" s="1" t="n">
-        <v>0.2336243711747108</v>
+        <v>0.2336243728742284</v>
       </c>
       <c r="C223" s="1" t="n">
         <v>0.1449319339258581</v>
@@ -3804,7 +3804,7 @@
         </is>
       </c>
       <c r="B224" s="1" t="n">
-        <v>0.2393671014245891</v>
+        <v>0.2393671031320184</v>
       </c>
       <c r="C224" s="1" t="n">
         <v>0.1460824939125074</v>
@@ -3817,7 +3817,7 @@
         </is>
       </c>
       <c r="B225" s="1" t="n">
-        <v>0.2448406553564695</v>
+        <v>0.2448406570714396</v>
       </c>
       <c r="C225" s="1" t="n">
         <v>0.1368177471994592</v>
@@ -3830,7 +3830,7 @@
         </is>
       </c>
       <c r="B226" s="1" t="n">
-        <v>0.2481449203473478</v>
+        <v>0.2481449220668701</v>
       </c>
       <c r="C226" s="1" t="n">
         <v>0.1545707945841823</v>
@@ -3843,7 +3843,7 @@
         </is>
       </c>
       <c r="B227" s="1" t="n">
-        <v>0.2466644617658331</v>
+        <v>0.2466644634833159</v>
       </c>
       <c r="C227" s="1" t="n">
         <v>0.1536057593628866</v>
@@ -3856,7 +3856,7 @@
         </is>
       </c>
       <c r="B228" s="1" t="n">
-        <v>0.259897738207058</v>
+        <v>0.2598977399427718</v>
       </c>
       <c r="C228" s="1" t="n">
         <v>0.1756108096457798</v>
@@ -3869,7 +3869,7 @@
         </is>
       </c>
       <c r="B229" s="1" t="n">
-        <v>0.2646590105172</v>
+        <v>0.2646590122594732</v>
       </c>
       <c r="C229" s="1" t="n">
         <v>0.17748827430494</v>
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="B230" s="1" t="n">
-        <v>0.2664925940380356</v>
+        <v>0.266492595782835</v>
       </c>
       <c r="C230" s="1" t="n">
         <v>0.1788899886022917</v>
@@ -3895,7 +3895,7 @@
         </is>
       </c>
       <c r="B231" s="1" t="n">
-        <v>0.2733255801557524</v>
+        <v>0.2733255819099654</v>
       </c>
       <c r="C231" s="1" t="n">
         <v>0.1804013834044187</v>
@@ -3908,7 +3908,7 @@
         </is>
       </c>
       <c r="B232" s="1" t="n">
-        <v>0.278916029050192</v>
+        <v>0.2789160308121068</v>
       </c>
       <c r="C232" s="1" t="n">
         <v>0.1891248778942503</v>
@@ -3921,7 +3921,7 @@
         </is>
       </c>
       <c r="B233" s="1" t="n">
-        <v>0.2786312350299895</v>
+        <v>0.278631236791512</v>
       </c>
       <c r="C233" s="1" t="n">
         <v>0.1867217384525981</v>
@@ -3934,7 +3934,7 @@
         </is>
       </c>
       <c r="B234" s="1" t="n">
-        <v>0.288455692705613</v>
+        <v>0.2884556944806702</v>
       </c>
       <c r="C234" s="1" t="n">
         <v>0.1915411687817603</v>
@@ -3947,7 +3947,7 @@
         </is>
       </c>
       <c r="B235" s="1" t="n">
-        <v>0.2896513538135743</v>
+        <v>0.2896513555902787</v>
       </c>
       <c r="C235" s="1" t="n">
         <v>0.1915411687817603</v>
@@ -3960,7 +3960,7 @@
         </is>
       </c>
       <c r="B236" s="1" t="n">
-        <v>0.2918149381039579</v>
+        <v>0.2918149398836429</v>
       </c>
       <c r="C236" s="1" t="n">
         <v>0.192252368329606</v>
@@ -3973,7 +3973,7 @@
         </is>
       </c>
       <c r="B237" s="1" t="n">
-        <v>0.2854077883520449</v>
+        <v>0.2854077901229031</v>
       </c>
       <c r="C237" s="1" t="n">
         <v>0.1899225194697247</v>
@@ -3986,7 +3986,7 @@
         </is>
       </c>
       <c r="B238" s="1" t="n">
-        <v>0.2866441419353607</v>
+        <v>0.2866441437079221</v>
       </c>
       <c r="C238" s="1" t="n">
         <v>0.1910887845810392</v>
@@ -3999,7 +3999,7 @@
         </is>
       </c>
       <c r="B239" s="1" t="n">
-        <v>0.2894372462324153</v>
+        <v>0.2894372480088245</v>
       </c>
       <c r="C239" s="1" t="n">
         <v>0.1899617184394173</v>
@@ -4012,7 +4012,7 @@
         </is>
       </c>
       <c r="B240" s="1" t="n">
-        <v>0.3017883197193223</v>
+        <v>0.301788321512747</v>
       </c>
       <c r="C240" s="1" t="n">
         <v>0.194464620280409</v>
@@ -4025,7 +4025,7 @@
         </is>
       </c>
       <c r="B241" s="1" t="n">
-        <v>0.3017883197193223</v>
+        <v>0.301788321512747</v>
       </c>
       <c r="C241" s="1" t="n">
         <v>0.194464620280409</v>
@@ -4057,9 +4057,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.3" customWidth="1" min="1" max="1"/>
-    <col width="30.59" customWidth="1" min="2" max="2"/>
+    <col width="29.26" customWidth="1" min="2" max="2"/>
     <col width="29.26" customWidth="1" min="3" max="3"/>
-    <col width="29.26" customWidth="1" min="4" max="4"/>
+    <col width="30.59" customWidth="1" min="4" max="4"/>
     <col width="30.59" customWidth="1" min="5" max="5"/>
     <col width="30.59" customWidth="1" min="6" max="6"/>
     <col width="30.59" customWidth="1" min="7" max="7"/>
@@ -4165,7 +4165,7 @@
         <v>0.03375085031185554</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>-0.04374322677499454</v>
+        <v>-0.04374316252051802</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>0.01726045181352398</v>
@@ -4190,7 +4190,7 @@
         <v>0.0006732342514317313</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>-0.02963768392020694</v>
+        <v>-0.02963774912248329</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>-0.002888076797592731</v>
@@ -4209,13 +4209,13 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.03679406207969693</v>
+        <v>0.03679418481268826</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.009418080144487861</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.01178539904311671</v>
+        <v>0.01178526055103646</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>0.005611780984804415</v>
@@ -4234,13 +4234,13 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0.004088755590669013</v>
+        <v>0.004088755106652631</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0.01432856331507937</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0.009736196703203026</v>
+        <v>0.009736403354272838</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>0.004680566980618694</v>
@@ -4259,13 +4259,13 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.004456562515547491</v>
+        <v>0.004456444094792955</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>-0.006570309520439799</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.00761720014247258</v>
+        <v>0.007617131846648029</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>-0.002150267670138928</v>
@@ -4315,7 +4315,7 @@
         <v>0.008737851559167842</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0.01162140274951962</v>
+        <v>0.0116214680423341</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>0.005310647742021946</v>
@@ -4334,13 +4334,13 @@
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.01011920097164198</v>
+        <v>0.01011908595719624</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>-0.006737251777299891</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.003018728366081191</v>
+        <v>0.003018728171244156</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>0.003345661085441876</v>
@@ -4384,13 +4384,13 @@
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.008756234812199004</v>
+        <v>0.008756235809203705</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.01315368503983905</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.004681802846403738</v>
+        <v>0.004681673848171863</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>-0.005035634587212789</v>
@@ -4409,13 +4409,13 @@
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>-0.005369975813380612</v>
+        <v>-0.005369863545597653</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>-0.005383169206004901</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>-0.01888922009143834</v>
+        <v>-0.01888915725263929</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>-0.01884815552300056</v>
@@ -4440,7 +4440,7 @@
         <v>-0.02324099164597015</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>-0.01645387211488958</v>
+        <v>-0.01645393739663448</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>-0.001067258371973634</v>
@@ -4459,13 +4459,13 @@
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.01922064970095105</v>
+        <v>0.01922076313392163</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.01271188175538818</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>0.03574358028786873</v>
+        <v>0.03574358266030786</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>-0.002492860441840383</v>
@@ -4484,13 +4484,13 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.02350058273449829</v>
+        <v>0.02350046882521029</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.01609267996954955</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>0.009824288116401902</v>
+        <v>0.009824352829264527</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>0.01017494261084195</v>
@@ -4515,7 +4515,7 @@
         <v>-0.0009502609720638544</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>-0.002226044196731114</v>
+        <v>-0.002226107656569054</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>-0.005478046040928386</v>
@@ -4534,13 +4534,13 @@
         </is>
       </c>
       <c r="B19" s="1" t="n">
-        <v>-0.004700651582395188</v>
+        <v>-0.004700759237479035</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>-0.004121776478443695</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>-0.005908126480323017</v>
+        <v>-0.00590806325466664</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>0.001243807390044926</v>
@@ -4559,13 +4559,13 @@
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>0.01480336790924563</v>
+        <v>0.01480347767396473</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.01337154655965356</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>0.03071363856249265</v>
+        <v>0.03071357458307644</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>-0.02573201961697758</v>
@@ -4584,13 +4584,13 @@
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>0.01368421770682571</v>
+        <v>0.0136841111211301</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0.003141724576239291</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>0.0006451860394005582</v>
+        <v>0.0006452481523835374</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>-0.002367920389281686</v>
@@ -4609,13 +4609,13 @@
         </is>
       </c>
       <c r="B22" s="1" t="n">
-        <v>-0.02007800003133375</v>
+        <v>-0.02007800214247235</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0.003131823587420035</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>-0.02196169641640855</v>
+        <v>-0.02196163438350085</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>0.01497165814838963</v>
@@ -4634,13 +4634,13 @@
         </is>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.009020815045178709</v>
+        <v>0.009020923314372542</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>-0.008741789769947217</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>0.02101272937719689</v>
+        <v>0.02101260119276094</v>
       </c>
       <c r="E23" s="1" t="n">
         <v>0.002698384032325585</v>
@@ -4659,13 +4659,13 @@
         </is>
       </c>
       <c r="B24" s="1" t="n">
-        <v>0.007900781262378809</v>
+        <v>0.007900674920432227</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>0.006929135279573284</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>0.01993466287408441</v>
+        <v>0.01993466411243627</v>
       </c>
       <c r="E24" s="1" t="n">
         <v>-0.004126387604476256</v>
@@ -4684,13 +4684,13 @@
         </is>
       </c>
       <c r="B25" s="1" t="n">
-        <v>0.03706265602706416</v>
+        <v>0.03706276544584353</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>-0.02783860156670293</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>0.0468842672859302</v>
+        <v>0.04688433104786194</v>
       </c>
       <c r="E25" s="1" t="n">
         <v>-0.01080880986821442</v>
@@ -4709,13 +4709,13 @@
         </is>
       </c>
       <c r="B26" s="1" t="n">
-        <v>0.02439974769055464</v>
+        <v>0.02439984942823425</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>0.02573999087361112</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>-0.02362067294383929</v>
+        <v>-0.02362055658641771</v>
       </c>
       <c r="E26" s="1" t="n">
         <v>0.01784740679249985</v>
@@ -4734,13 +4734,13 @@
         </is>
       </c>
       <c r="B27" s="1" t="n">
-        <v>-0.01792873792212357</v>
+        <v>-0.01792873614154133</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>-0.01411537190695245</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>-0.006115686799802789</v>
+        <v>-0.006115864829490003</v>
       </c>
       <c r="E27" s="1" t="n">
         <v>-0.002683829806365612</v>
@@ -4759,13 +4759,13 @@
         </is>
       </c>
       <c r="B28" s="1" t="n">
-        <v>0.0192445673031465</v>
+        <v>0.01924466648450229</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>-0.0108177204241986</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>0.04202213698262214</v>
+        <v>0.04202195964347011</v>
       </c>
       <c r="E28" s="1" t="n">
         <v>-0.01291710640975141</v>
@@ -4784,13 +4784,13 @@
         </is>
       </c>
       <c r="B29" s="1" t="n">
-        <v>-0.01765268799227682</v>
+        <v>-0.01765278370743684</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>-0.01254418028529791</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>-0.00310206148198866</v>
+        <v>-0.003101947125707771</v>
       </c>
       <c r="E29" s="1" t="n">
         <v>0.003089708318388507</v>
@@ -4809,13 +4809,13 @@
         </is>
       </c>
       <c r="B30" s="1" t="n">
-        <v>-0.006911602970521735</v>
+        <v>-0.006911501271401166</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>0.01563517007359838</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>-0.0116598671744278</v>
+        <v>-0.01165975309206291</v>
       </c>
       <c r="E30" s="1" t="n">
         <v>-0.01250224544841494</v>
@@ -4834,7 +4834,7 @@
         </is>
       </c>
       <c r="B31" s="1" t="n">
-        <v>0.002456253046034584</v>
+        <v>0.002456150842444549</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>-0.008018015970818748</v>
@@ -4859,7 +4859,7 @@
         </is>
       </c>
       <c r="B32" s="1" t="n">
-        <v>0.01880687745793264</v>
+        <v>0.01880677409510456</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0.0109925952022758</v>
@@ -4915,7 +4915,7 @@
         <v>0.02057217345145324</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>-0.007993024499883039</v>
+        <v>-0.007992911378773226</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>-0.005390878992001524</v>
@@ -4934,13 +4934,13 @@
         </is>
       </c>
       <c r="B35" s="1" t="n">
-        <v>-0.01042946842654491</v>
+        <v>-0.01042936979340303</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>-0.007244093164233245</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>-0.02662261512272646</v>
+        <v>-0.02662272611944339</v>
       </c>
       <c r="E35" s="1" t="n">
         <v>-0.02529355535212141</v>
@@ -4959,13 +4959,13 @@
         </is>
       </c>
       <c r="B36" s="1" t="n">
-        <v>-0.007546616910067305</v>
+        <v>-0.007546715830540895</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>0.001269024470129443</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>-0.01560176191099327</v>
+        <v>-0.01560164475954018</v>
       </c>
       <c r="E36" s="1" t="n">
         <v>0.01278959983412564</v>
@@ -5015,7 +5015,7 @@
         <v>-0.008267080797670245</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>-0.02088659197791964</v>
+        <v>-0.02088670850042085</v>
       </c>
       <c r="E38" s="1" t="n">
         <v>0.0007303422174962382</v>
@@ -5034,13 +5034,13 @@
         </is>
       </c>
       <c r="B39" s="1" t="n">
-        <v>0.002895948107779711</v>
+        <v>0.002896051291279678</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>-0.004590947612986174</v>
+        <v>-0.004591008386431561</v>
       </c>
       <c r="E39" s="1" t="n">
         <v>0.00675059234514408</v>
@@ -5059,13 +5059,13 @@
         </is>
       </c>
       <c r="B40" s="1" t="n">
-        <v>0.003290588503280789</v>
+        <v>0.003290588164726715</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>0.006732868328391151</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>0.0129617700407223</v>
+        <v>0.01296177083208683</v>
       </c>
       <c r="E40" s="1" t="n">
         <v>-0.01540410178808027</v>
@@ -5084,13 +5084,13 @@
         </is>
       </c>
       <c r="B41" s="1" t="n">
-        <v>-0.01800529373827942</v>
+        <v>-0.01800539443996541</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>-0.01019105676497567</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>-0.02178441080676308</v>
+        <v>-0.02178429157475359</v>
       </c>
       <c r="E41" s="1" t="n">
         <v>-0.003129092142560408</v>
@@ -5115,7 +5115,7 @@
         <v>0.008687246130473003</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>0.003771808075992089</v>
+        <v>0.003771746228854456</v>
       </c>
       <c r="E42" s="1" t="n">
         <v>0.002954199821529668</v>
@@ -5140,7 +5140,7 @@
         <v>-0.00223283543367403</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>-0.002958118599495241</v>
+        <v>-0.002958179982712084</v>
       </c>
       <c r="E43" s="1" t="n">
         <v>-0.02356405790351346</v>
@@ -5159,13 +5159,13 @@
         </is>
       </c>
       <c r="B44" s="1" t="n">
-        <v>-0.01424592002687275</v>
+        <v>-0.01424602395934493</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>0.00607411582100581</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>-0.01262926642379958</v>
+        <v>-0.01262926720132473</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>-0.004524908581630571</v>
@@ -5184,13 +5184,13 @@
         </is>
       </c>
       <c r="B45" s="1" t="n">
-        <v>0.004129130672652082</v>
+        <v>0.004129131108004724</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>0.01965316751311641</v>
+        <v>0.01965323109135486</v>
       </c>
       <c r="E45" s="1" t="n">
         <v>0.02026513487839066</v>
@@ -5209,7 +5209,7 @@
         </is>
       </c>
       <c r="B46" s="1" t="n">
-        <v>0.03509004773971869</v>
+        <v>0.03509005142420629</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>0.007944067220718942</v>
@@ -5234,7 +5234,7 @@
         </is>
       </c>
       <c r="B47" s="1" t="n">
-        <v>0.01853941919152469</v>
+        <v>0.01853942107218831</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>0.005674665934060519</v>
@@ -5259,13 +5259,13 @@
         </is>
       </c>
       <c r="B48" s="1" t="n">
-        <v>-0.01449653678627549</v>
+        <v>-0.01449643863513927</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>-0.00532910737343828</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>-0.01058908705014461</v>
+        <v>-0.0105890272703888</v>
       </c>
       <c r="E48" s="1" t="n">
         <v>0.001714321882627434</v>
@@ -5290,7 +5290,7 @@
         <v>0.004727346099755447</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>-0.001770534306941962</v>
+        <v>-0.001770594619507015</v>
       </c>
       <c r="E49" s="1" t="n">
         <v>0.001331005141085528</v>
@@ -5359,13 +5359,13 @@
         </is>
       </c>
       <c r="B52" s="1" t="n">
-        <v>0.01326606399796471</v>
+        <v>0.01326596082835696</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>-0.02970616283862604</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>0.02144092340069759</v>
+        <v>0.02144086162980652</v>
       </c>
       <c r="E52" s="1" t="n">
         <v>0.01232698578282987</v>
@@ -5384,13 +5384,13 @@
         </is>
       </c>
       <c r="B53" s="1" t="n">
-        <v>0.01408918640815804</v>
+        <v>0.01408928966158562</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>0.02529115760784939</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>0.02705576374493912</v>
+        <v>0.02705594680392864</v>
       </c>
       <c r="E53" s="1" t="n">
         <v>0.003746727140466088</v>
@@ -5415,7 +5415,7 @@
         <v>-0.04868545214940845</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>0.01783040238464118</v>
+        <v>0.0178304002848908</v>
       </c>
       <c r="E54" s="1" t="n">
         <v>0.0007464898758908767</v>
@@ -5440,7 +5440,7 @@
         <v>0.02661211397806618</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>0.04053656298224961</v>
+        <v>0.04053644259279121</v>
       </c>
       <c r="E55" s="1" t="n">
         <v>0.02331217776024608</v>
@@ -5484,13 +5484,13 @@
         </is>
       </c>
       <c r="B57" s="1" t="n">
-        <v>0.01548387670702112</v>
+        <v>0.01548397555016101</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>0.0144927593754236</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>-0.02576654764860464</v>
+        <v>-0.02576665755539387</v>
       </c>
       <c r="E57" s="1" t="n">
         <v>-0.003292408516962886</v>
@@ -5509,13 +5509,13 @@
         </is>
       </c>
       <c r="B58" s="1" t="n">
-        <v>0.01194410071317109</v>
+        <v>0.01194400221458847</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>0.0182723960040907</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>0.005693589897045159</v>
+        <v>0.005693590539359583</v>
       </c>
       <c r="E58" s="1" t="n">
         <v>-0.009543092603295111</v>
@@ -5534,13 +5534,13 @@
         </is>
       </c>
       <c r="B59" s="1" t="n">
-        <v>-0.009103438776553507</v>
+        <v>-0.009103342589421137</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>0.008482861285229237</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>-0.005442278820206869</v>
+        <v>-0.005442279430694197</v>
       </c>
       <c r="E59" s="1" t="n">
         <v>0.01593482477828045</v>
@@ -5559,13 +5559,13 @@
         </is>
       </c>
       <c r="B60" s="1" t="n">
-        <v>0.006969490061793371</v>
+        <v>0.006969392314458034</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>-0.004852756232196276</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>0.0197215651650573</v>
+        <v>0.0197216801781972</v>
       </c>
       <c r="E60" s="1" t="n">
         <v>-0.0001824571322107671</v>
@@ -5609,13 +5609,13 @@
         </is>
       </c>
       <c r="B62" s="1" t="n">
-        <v>-0.01229335716062596</v>
+        <v>-0.01229326155571753</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>0.01658029463166044</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>-0.01493398454859707</v>
+        <v>-0.01493387508838917</v>
       </c>
       <c r="E62" s="1" t="n">
         <v>-0.0009120237631667916</v>
@@ -5634,13 +5634,13 @@
         </is>
       </c>
       <c r="B63" s="1" t="n">
-        <v>-0.00398030070092048</v>
+        <v>-0.003980300315648</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>0.01087324809738255</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>-0.004160764823335827</v>
+        <v>-0.004160986600303063</v>
       </c>
       <c r="E63" s="1" t="n">
         <v>0.00657293703335271</v>
@@ -5659,13 +5659,13 @@
         </is>
       </c>
       <c r="B64" s="1" t="n">
-        <v>0.0197907523492693</v>
+        <v>0.01979084760761629</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>0.01109243441028762</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>0.01918384603736967</v>
+        <v>0.01918395976193343</v>
       </c>
       <c r="E64" s="1" t="n">
         <v>0.0157808593255806</v>
@@ -5684,7 +5684,7 @@
         </is>
       </c>
       <c r="B65" s="1" t="n">
-        <v>0.009889881075754836</v>
+        <v>0.009889783895166371</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>0.02460105628308096</v>
@@ -5709,7 +5709,7 @@
         </is>
       </c>
       <c r="B66" s="1" t="n">
-        <v>0.01564425583697782</v>
+        <v>0.01564425436074779</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>0.01784559214325832</v>
@@ -5734,13 +5734,13 @@
         </is>
       </c>
       <c r="B67" s="1" t="n">
-        <v>0.007701687923461709</v>
+        <v>0.007701687207905872</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>0.00031872238653885</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>-0.003711342754008085</v>
+        <v>-0.003711236228670645</v>
       </c>
       <c r="E67" s="1" t="n">
         <v>0.0057420213651318</v>
@@ -5759,13 +5759,13 @@
         </is>
       </c>
       <c r="B68" s="1" t="n">
-        <v>-0.003249641346398491</v>
+        <v>-0.003249733245646036</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>-0.01306564239570529</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>-0.0001740692800010768</v>
+        <v>-0.0001741761835399869</v>
       </c>
       <c r="E68" s="1" t="n">
         <v>-0.007136496119925617</v>
@@ -5790,7 +5790,7 @@
         <v>-0.02970617038074119</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>-0.009889241436984664</v>
+        <v>-0.009889348377761897</v>
       </c>
       <c r="E69" s="1" t="n">
         <v>0.01383641827155535</v>
@@ -5809,13 +5809,13 @@
         </is>
       </c>
       <c r="B70" s="1" t="n">
-        <v>0.005496025004078975</v>
+        <v>0.005495931448347591</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>-0.005989963474114068</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>0.02553276471686106</v>
+        <v>0.02553298349245736</v>
       </c>
       <c r="E70" s="1" t="n">
         <v>0.007798748595647442</v>
@@ -5859,13 +5859,13 @@
         </is>
       </c>
       <c r="B72" s="1" t="n">
-        <v>-0.01597245961456184</v>
+        <v>-0.01597236805634317</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>-0.007578812647770272</v>
+        <v>-0.00757891716935799</v>
       </c>
       <c r="E72" s="1" t="n">
         <v>0</v>
@@ -5909,13 +5909,13 @@
         </is>
       </c>
       <c r="B74" s="1" t="n">
-        <v>-0.004353151706989244</v>
+        <v>-0.004353246984883374</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>0.01272013671198224</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>0.002333503595485009</v>
+        <v>0.002333612181040889</v>
       </c>
       <c r="E74" s="1" t="n">
         <v>-0.004232009181523333</v>
@@ -5934,13 +5934,13 @@
         </is>
       </c>
       <c r="B75" s="1" t="n">
-        <v>0.03410349835046667</v>
+        <v>0.03410359730845891</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>-0.006763255704754001</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>0.02239942332304667</v>
+        <v>0.02239931256370653</v>
       </c>
       <c r="E75" s="1" t="n">
         <v>-0.01168759076672987</v>
@@ -6034,13 +6034,13 @@
         </is>
       </c>
       <c r="B79" s="1" t="n">
-        <v>0.006968164597188409</v>
+        <v>0.006968256629898306</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>-0.008477251319618739</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>0.0002774311219995163</v>
+        <v>0.0002775376214705361</v>
       </c>
       <c r="E79" s="1" t="n">
         <v>0.002631565756218368</v>
@@ -6059,13 +6059,13 @@
         </is>
       </c>
       <c r="B80" s="1" t="n">
-        <v>-0.00584613545449697</v>
+        <v>-0.005846409107705175</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>-0.001583256402195699</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>-0.008112370070748165</v>
+        <v>-0.008112475676946396</v>
       </c>
       <c r="E80" s="1" t="n">
         <v>0.003849463038669176</v>
@@ -6084,13 +6084,13 @@
         </is>
       </c>
       <c r="B81" s="1" t="n">
-        <v>-0.009780967985973943</v>
+        <v>-0.009780785917727575</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>0.00126860156383235</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>-0.001223147511160483</v>
+        <v>-0.001223254851881128</v>
       </c>
       <c r="E81" s="1" t="n">
         <v>0.0135960389487455</v>
@@ -6109,13 +6109,13 @@
         </is>
       </c>
       <c r="B82" s="1" t="n">
-        <v>0.001878459676063482</v>
+        <v>0.001878552517445176</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>0.003167576257091964</v>
       </c>
       <c r="D82" s="1" t="n">
-        <v>-0.01396289243733351</v>
+        <v>-0.01396289393795613</v>
       </c>
       <c r="E82" s="1" t="n">
         <v>0.01155710179139646</v>
@@ -6134,13 +6134,13 @@
         </is>
       </c>
       <c r="B83" s="1" t="n">
-        <v>-0.0094356634960856</v>
+        <v>-0.009435755289009418</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>0.03504890117868364</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>-0.02253604514882213</v>
+        <v>-0.02253593861105818</v>
       </c>
       <c r="E83" s="1" t="n">
         <v>0.007500374616168148</v>
@@ -6209,13 +6209,13 @@
         </is>
       </c>
       <c r="B86" s="1" t="n">
-        <v>0.007541077740766067</v>
+        <v>0.007540986768225899</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>-0.004031040871790181</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>0.007971747622681269</v>
+        <v>0.007971646873896177</v>
       </c>
       <c r="E86" s="1" t="n">
         <v>0.007211958811199404</v>
@@ -6234,13 +6234,13 @@
         </is>
       </c>
       <c r="B87" s="1" t="n">
-        <v>-0.0005303731157714209</v>
+        <v>-0.0005303731636596698</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>-0.00553284257571085</v>
+        <v>-0.005532743176726584</v>
       </c>
       <c r="E87" s="1" t="n">
         <v>0</v>
@@ -6259,13 +6259,13 @@
         </is>
       </c>
       <c r="B88" s="1" t="n">
-        <v>-0.006191421572435907</v>
+        <v>-0.006191422131766267</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>-0.00591527500084621</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>-0.0004909820122683817</v>
+        <v>-0.0004908815041799741</v>
       </c>
       <c r="E88" s="1" t="n">
         <v>0.0003492919725802679</v>
@@ -6284,13 +6284,13 @@
         </is>
       </c>
       <c r="B89" s="1" t="n">
-        <v>-0.006467340186584347</v>
+        <v>-0.006467249872100345</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>0.003758187620978903</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>-0.003306932642490157</v>
+        <v>-0.003307133424854003</v>
       </c>
       <c r="E89" s="1" t="n">
         <v>0.01361736401216662</v>
@@ -6315,7 +6315,7 @@
         <v>-0.009984390091784867</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>0.003317904729946308</v>
+        <v>0.003318106846914581</v>
       </c>
       <c r="E90" s="1" t="n">
         <v>-0.004478162764048332</v>
@@ -6340,7 +6340,7 @@
         <v>0.009769977238050842</v>
       </c>
       <c r="D91" s="1" t="n">
-        <v>0.01715731500720552</v>
+        <v>0.01715721272445925</v>
       </c>
       <c r="E91" s="1" t="n">
         <v>0.007439451744837955</v>
@@ -6365,7 +6365,7 @@
         <v>0.005617986892395788</v>
       </c>
       <c r="D92" s="1" t="n">
-        <v>-0.006438043397130166</v>
+        <v>-0.006438142258396673</v>
       </c>
       <c r="E92" s="1" t="n">
         <v>-0.000686946863159954</v>
@@ -6390,7 +6390,7 @@
         <v>0.009621277059249644</v>
       </c>
       <c r="D93" s="1" t="n">
-        <v>-0.005345837135548259</v>
+        <v>-0.00534593716934284</v>
       </c>
       <c r="E93" s="1" t="n">
         <v>0.0003437095417715419</v>
@@ -6415,7 +6415,7 @@
         <v>0.002151850521087795</v>
       </c>
       <c r="D94" s="1" t="n">
-        <v>0.01729623561110438</v>
+        <v>0.01729643914494661</v>
       </c>
       <c r="E94" s="1" t="n">
         <v>-0.01580481332099382</v>
@@ -6434,7 +6434,7 @@
         </is>
       </c>
       <c r="B95" s="1" t="n">
-        <v>0.001094763513602937</v>
+        <v>0.00109485178674551</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>0.01042945302153298</v>
@@ -6459,7 +6459,7 @@
         </is>
       </c>
       <c r="B96" s="1" t="n">
-        <v>-0.00541757091780215</v>
+        <v>-0.005417570440099162</v>
       </c>
       <c r="C96" s="1" t="n">
         <v>0.005464490366730912</v>
@@ -6484,13 +6484,13 @@
         </is>
       </c>
       <c r="B97" s="1" t="n">
-        <v>-0.002897307985966657</v>
+        <v>-0.002897396386007611</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>-0.0006038785751414366</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>0.001585908110565581</v>
+        <v>0.001585808711749515</v>
       </c>
       <c r="E97" s="1" t="n">
         <v>-0.001043683623921154</v>
@@ -6515,7 +6515,7 @@
         <v>-0.005135896579518739</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>0.007367683636587019</v>
+        <v>0.007367783609204759</v>
       </c>
       <c r="E98" s="1" t="n">
         <v>-0.003482513701491774</v>
@@ -6559,7 +6559,7 @@
         </is>
       </c>
       <c r="B100" s="1" t="n">
-        <v>0.01366600279252395</v>
+        <v>0.01366609138782771</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>0</v>
@@ -6584,7 +6584,7 @@
         </is>
       </c>
       <c r="B101" s="1" t="n">
-        <v>0.0006284997498586797</v>
+        <v>0.0006284122940518611</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>0.02293988219229592</v>
@@ -6709,7 +6709,7 @@
         </is>
       </c>
       <c r="B106" s="1" t="n">
-        <v>0.01410485360781855</v>
+        <v>0.01410476516615367</v>
       </c>
       <c r="C106" s="1" t="n">
         <v>0.01567210527368679</v>
@@ -6759,7 +6759,7 @@
         </is>
       </c>
       <c r="B108" s="1" t="n">
-        <v>0.0106595199701387</v>
+        <v>0.01065960811133837</v>
       </c>
       <c r="C108" s="1" t="n">
         <v>-0.0002967992879533421</v>
@@ -6784,7 +6784,7 @@
         </is>
       </c>
       <c r="B109" s="1" t="n">
-        <v>-0.0002820013744546657</v>
+        <v>-0.0002820876661849825</v>
       </c>
       <c r="C109" s="1" t="n">
         <v>-0.0127634408638676</v>
@@ -6809,7 +6809,7 @@
         </is>
       </c>
       <c r="B110" s="1" t="n">
-        <v>0.01602250708827579</v>
+        <v>0.01602259478735468</v>
       </c>
       <c r="C110" s="1" t="n">
         <v>0.007817262457952001</v>
@@ -6884,7 +6884,7 @@
         </is>
       </c>
       <c r="B113" s="1" t="n">
-        <v>-0.002060298425064055</v>
+        <v>-0.002060383621211082</v>
       </c>
       <c r="C113" s="1" t="n">
         <v>0.002063062015756678</v>
@@ -6909,7 +6909,7 @@
         </is>
       </c>
       <c r="B114" s="1" t="n">
-        <v>-0.007756305856257195</v>
+        <v>-0.007756221146382636</v>
       </c>
       <c r="C114" s="1" t="n">
         <v>0.002941131591796875</v>
@@ -6984,7 +6984,7 @@
         </is>
       </c>
       <c r="B117" s="1" t="n">
-        <v>0.01563880881166679</v>
+        <v>0.01563872426522583</v>
       </c>
       <c r="C117" s="1" t="n">
         <v>0.008985547051913567</v>
@@ -7009,7 +7009,7 @@
         </is>
       </c>
       <c r="B118" s="1" t="n">
-        <v>-0.002611715910839085</v>
+        <v>-0.002611549639047195</v>
       </c>
       <c r="C118" s="1" t="n">
         <v>0.01350179222820946</v>
@@ -7034,7 +7034,7 @@
         </is>
       </c>
       <c r="B119" s="1" t="n">
-        <v>0.003491406442876821</v>
+        <v>0.003491322688906839</v>
       </c>
       <c r="C119" s="1" t="n">
         <v>0.003684837659107876</v>
@@ -7059,7 +7059,7 @@
         </is>
       </c>
       <c r="B120" s="1" t="n">
-        <v>0.01119871914831672</v>
+        <v>0.01119863597612958</v>
       </c>
       <c r="C120" s="1" t="n">
         <v>0.00169447538970835</v>
@@ -7084,7 +7084,7 @@
         </is>
       </c>
       <c r="B121" s="1" t="n">
-        <v>-0.005859978228138996</v>
+        <v>-0.005859896459041392</v>
       </c>
       <c r="C121" s="1" t="n">
         <v>0.0005638696666296905</v>
@@ -7184,7 +7184,7 @@
         </is>
       </c>
       <c r="B125" s="1" t="n">
-        <v>0.01652524837190983</v>
+        <v>0.01652533153957325</v>
       </c>
       <c r="C125" s="1" t="n">
         <v>-0.005196313751367199</v>
@@ -7209,7 +7209,7 @@
         </is>
       </c>
       <c r="B126" s="1" t="n">
-        <v>-0.001711255917520638</v>
+        <v>-0.001711337593146123</v>
       </c>
       <c r="C126" s="1" t="n">
         <v>-0.004643060117903608</v>
@@ -7234,7 +7234,7 @@
         </is>
       </c>
       <c r="B127" s="1" t="n">
-        <v>-0.007552972597393515</v>
+        <v>-0.007552890641506438</v>
       </c>
       <c r="C127" s="1" t="n">
         <v>0.002332414951433881</v>
@@ -7259,7 +7259,7 @@
         </is>
       </c>
       <c r="B128" s="1" t="n">
-        <v>0.01505905226521231</v>
+        <v>0.01505896844203991</v>
       </c>
       <c r="C128" s="1" t="n">
         <v>0.01076203956921651</v>
@@ -7334,7 +7334,7 @@
         </is>
       </c>
       <c r="B131" s="1" t="n">
-        <v>0.02310253288280206</v>
+        <v>0.02310261358075549</v>
       </c>
       <c r="C131" s="1" t="n">
         <v>0.02059759383026138</v>
@@ -7359,7 +7359,7 @@
         </is>
       </c>
       <c r="B132" s="1" t="n">
-        <v>-0.007784639615237898</v>
+        <v>-0.00778471787693702</v>
       </c>
       <c r="C132" s="1" t="n">
         <v>-0.01620237890504961</v>
@@ -7509,7 +7509,7 @@
         </is>
       </c>
       <c r="B138" s="1" t="n">
-        <v>-0.002810063567528331</v>
+        <v>-0.002809982450284298</v>
       </c>
       <c r="C138" s="1" t="n">
         <v>0.002680969717189674</v>
@@ -7534,7 +7534,7 @@
         </is>
       </c>
       <c r="B139" s="1" t="n">
-        <v>0.008985541836038946</v>
+        <v>0.008985459759278225</v>
       </c>
       <c r="C139" s="1" t="n">
         <v>0.01633984668906141</v>
@@ -7559,7 +7559,7 @@
         </is>
       </c>
       <c r="B140" s="1" t="n">
-        <v>0.004057514019659036</v>
+        <v>0.004057433398255039</v>
       </c>
       <c r="C140" s="1" t="n">
         <v>-0.005846266246473886</v>
@@ -7584,7 +7584,7 @@
         </is>
       </c>
       <c r="B141" s="1" t="n">
-        <v>0.000787298391791369</v>
+        <v>0.0007872984550081341</v>
       </c>
       <c r="C141" s="1" t="n">
         <v>0.002646285122893</v>
@@ -7609,7 +7609,7 @@
         </is>
       </c>
       <c r="B142" s="1" t="n">
-        <v>0.01730549471039589</v>
+        <v>0.01730565656374394</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>-0.006158331198519718</v>
@@ -7634,7 +7634,7 @@
         </is>
       </c>
       <c r="B143" s="1" t="n">
-        <v>-0.001340275889884723</v>
+        <v>-0.001340354651768072</v>
       </c>
       <c r="C143" s="1" t="n">
         <v>0.004130994162578894</v>
@@ -7759,7 +7759,7 @@
         </is>
       </c>
       <c r="B148" s="1" t="n">
-        <v>0.004513577920933098</v>
+        <v>0.004513657295896589</v>
       </c>
       <c r="C148" s="1" t="n">
         <v>0.001424588431098606</v>
@@ -7784,7 +7784,7 @@
         </is>
       </c>
       <c r="B149" s="1" t="n">
-        <v>0.004545054066301901</v>
+        <v>0.004544974688857506</v>
       </c>
       <c r="C149" s="1" t="n">
         <v>-0.01308685289334188</v>
@@ -7909,7 +7909,7 @@
         </is>
       </c>
       <c r="B154" s="1" t="n">
-        <v>-0.01548997623454629</v>
+        <v>-0.01549005444897344</v>
       </c>
       <c r="C154" s="1" t="n">
         <v>-0.002868682933661937</v>
@@ -7934,7 +7934,7 @@
         </is>
       </c>
       <c r="B155" s="1" t="n">
-        <v>-0.007321653854831633</v>
+        <v>-0.007321574991465574</v>
       </c>
       <c r="C155" s="1" t="n">
         <v>-0.01467198924509927</v>
@@ -8034,7 +8034,7 @@
         </is>
       </c>
       <c r="B159" s="1" t="n">
-        <v>-0.008954306412041091</v>
+        <v>-0.008954391503947501</v>
       </c>
       <c r="C159" s="1" t="n">
         <v>0.007615762767392065</v>
@@ -8059,7 +8059,7 @@
         </is>
       </c>
       <c r="B160" s="1" t="n">
-        <v>-0.001234677294164377</v>
+        <v>-0.001234591539437502</v>
       </c>
       <c r="C160" s="1" t="n">
         <v>-0.02180232461431086</v>

</xml_diff>